<commit_message>
added all existing tests to matrix
</commit_message>
<xml_diff>
--- a/TraceabilityMatrix.xlsx
+++ b/TraceabilityMatrix.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rwilkins\Documents\GitHub\med656\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26423"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="10780" yWindow="0" windowWidth="20600" windowHeight="14240"/>
   </bookViews>
   <sheets>
     <sheet name="TraceabilityMatrix" sheetId="1" r:id="rId1"/>
@@ -22,12 +17,17 @@
     <definedName name="_Toc436595569" localSheetId="0">TraceabilityMatrix!#REF!</definedName>
     <definedName name="_Toc436595570" localSheetId="0">TraceabilityMatrix!$B$94</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="229">
   <si>
     <t>software design plan item</t>
   </si>
@@ -627,13 +627,100 @@
   </si>
   <si>
     <t>test plan title</t>
+  </si>
+  <si>
+    <t>5.2.1.11</t>
+  </si>
+  <si>
+    <t>5.2.1.10</t>
+  </si>
+  <si>
+    <t>5.2.1.12</t>
+  </si>
+  <si>
+    <t>5.2.1.13</t>
+  </si>
+  <si>
+    <t>5.2.1.14</t>
+  </si>
+  <si>
+    <t>5.2.1.15</t>
+  </si>
+  <si>
+    <t>5.2.1.16</t>
+  </si>
+  <si>
+    <t>5.2.1.17</t>
+  </si>
+  <si>
+    <t>5.2.1.18</t>
+  </si>
+  <si>
+    <t>5.2.1.19</t>
+  </si>
+  <si>
+    <t>User Login Customer Acceptance Tests</t>
+  </si>
+  <si>
+    <t>User Information Tests</t>
+  </si>
+  <si>
+    <t>User Privacy Tests</t>
+  </si>
+  <si>
+    <t>Account editing Tests</t>
+  </si>
+  <si>
+    <t>Account Management Tests</t>
+  </si>
+  <si>
+    <t>Username Tests</t>
+  </si>
+  <si>
+    <t>Patient ID Tests</t>
+  </si>
+  <si>
+    <t>Password Tests</t>
+  </si>
+  <si>
+    <t>Username/Password Retrieval Tests</t>
+  </si>
+  <si>
+    <t>Data File Processing Interface Tests</t>
+  </si>
+  <si>
+    <t>File Upload Interface Tests</t>
+  </si>
+  <si>
+    <t>Data Type Tests</t>
+  </si>
+  <si>
+    <t>Database Function Test</t>
+  </si>
+  <si>
+    <t>Experiment Tests</t>
+  </si>
+  <si>
+    <t>Data Exportation Tests</t>
+  </si>
+  <si>
+    <t>Medical Data View Tests</t>
+  </si>
+  <si>
+    <t>OS Test</t>
+  </si>
+  <si>
+    <t>SQL Database Test</t>
+  </si>
+  <si>
+    <t>Network Connection Test</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -767,6 +854,33 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
     </font>
   </fonts>
   <fills count="33">
@@ -950,7 +1064,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -1065,8 +1179,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF9BC2E6"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF9BC2E6"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1109,8 +1234,28 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1119,8 +1264,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="62">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1149,11 +1298,31 @@
     <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="50" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="52" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="54" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="56" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1165,23 +1334,6 @@
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="8">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1308,6 +1460,23 @@
       </font>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1322,15 +1491,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F93" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F93" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <autoFilter ref="A1:F93"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="requirement index" dataDxfId="7"/>
-    <tableColumn id="2" name="requirement description" dataDxfId="6"/>
-    <tableColumn id="3" name="test plan index" dataDxfId="5"/>
-    <tableColumn id="4" name="test plan title" dataDxfId="4"/>
-    <tableColumn id="5" name="test plan description" dataDxfId="3"/>
-    <tableColumn id="6" name="software design plan item" dataDxfId="2"/>
+    <tableColumn id="1" name="requirement index" dataDxfId="5"/>
+    <tableColumn id="2" name="requirement description" dataDxfId="4"/>
+    <tableColumn id="3" name="test plan index" dataDxfId="3"/>
+    <tableColumn id="4" name="test plan title" dataDxfId="2"/>
+    <tableColumn id="5" name="test plan description" dataDxfId="1"/>
+    <tableColumn id="6" name="software design plan item" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1379,7 +1548,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1414,7 +1583,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1591,7 +1760,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1601,21 +1770,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection sqref="A1:F93"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" customWidth="1"/>
-    <col min="2" max="2" width="85.28515625" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" customWidth="1"/>
+    <col min="1" max="1" width="19.83203125" customWidth="1"/>
+    <col min="2" max="2" width="85.33203125" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="5" max="5" width="21.28515625" customWidth="1"/>
-    <col min="6" max="6" width="26.140625" customWidth="1"/>
+    <col min="5" max="5" width="21.33203125" customWidth="1"/>
+    <col min="6" max="6" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -1635,7 +1804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15">
       <c r="A2" t="s">
         <v>175</v>
       </c>
@@ -1645,8 +1814,11 @@
       <c r="C2" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D2" s="5" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15">
       <c r="A3" t="s">
         <v>177</v>
       </c>
@@ -1656,8 +1828,11 @@
       <c r="C3" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D3" s="5" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>180</v>
       </c>
@@ -1667,8 +1842,11 @@
       <c r="C4" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="1" customFormat="1" ht="28">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -1678,11 +1856,13 @@
       <c r="C5" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="D5" s="3"/>
+      <c r="D5" s="5" t="s">
+        <v>211</v>
+      </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" s="1" customFormat="1" ht="15">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
@@ -1692,11 +1872,13 @@
       <c r="C6" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="D6" s="3"/>
+      <c r="D6" s="5" t="s">
+        <v>212</v>
+      </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" s="1" customFormat="1" ht="15">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -1706,11 +1888,13 @@
       <c r="C7" t="s">
         <v>189</v>
       </c>
-      <c r="D7"/>
+      <c r="D7" s="5" t="s">
+        <v>210</v>
+      </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" s="1" customFormat="1">
       <c r="A8" s="3" t="s">
         <v>181</v>
       </c>
@@ -1720,11 +1904,13 @@
       <c r="C8" t="s">
         <v>190</v>
       </c>
-      <c r="D8"/>
+      <c r="D8" t="s">
+        <v>190</v>
+      </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="1:6" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" s="1" customFormat="1" ht="28">
       <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
@@ -1734,11 +1920,13 @@
       <c r="C9" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="D9" s="3"/>
+      <c r="D9" s="5" t="s">
+        <v>211</v>
+      </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" s="1" customFormat="1" ht="28">
       <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
@@ -1748,11 +1936,13 @@
       <c r="C10" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="D10" s="3"/>
+      <c r="D10" s="5" t="s">
+        <v>213</v>
+      </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
     </row>
-    <row r="11" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" s="1" customFormat="1">
       <c r="A11" s="3" t="s">
         <v>12</v>
       </c>
@@ -1764,7 +1954,7 @@
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
     </row>
-    <row r="12" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" s="1" customFormat="1" ht="15">
       <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
@@ -1774,11 +1964,13 @@
       <c r="C12" t="s">
         <v>189</v>
       </c>
-      <c r="D12"/>
+      <c r="D12" s="5" t="s">
+        <v>210</v>
+      </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
     </row>
-    <row r="13" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" s="1" customFormat="1" ht="15">
       <c r="A13" s="3" t="s">
         <v>14</v>
       </c>
@@ -1788,11 +1980,13 @@
       <c r="C13" t="s">
         <v>189</v>
       </c>
-      <c r="D13"/>
+      <c r="D13" s="5" t="s">
+        <v>210</v>
+      </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
     </row>
-    <row r="14" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" s="1" customFormat="1" ht="15">
       <c r="A14" s="3" t="s">
         <v>15</v>
       </c>
@@ -1802,11 +1996,13 @@
       <c r="C14" t="s">
         <v>189</v>
       </c>
-      <c r="D14"/>
+      <c r="D14" s="5" t="s">
+        <v>210</v>
+      </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
     </row>
-    <row r="15" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" s="1" customFormat="1">
       <c r="A15" s="3" t="s">
         <v>183</v>
       </c>
@@ -1816,11 +2012,13 @@
       <c r="C15" t="s">
         <v>190</v>
       </c>
-      <c r="D15"/>
+      <c r="D15" t="s">
+        <v>190</v>
+      </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
     </row>
-    <row r="16" spans="1:6" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" s="1" customFormat="1" ht="28">
       <c r="A16" s="3" t="s">
         <v>21</v>
       </c>
@@ -1830,11 +2028,13 @@
       <c r="C16" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="D16" s="3"/>
+      <c r="D16" s="5" t="s">
+        <v>211</v>
+      </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
     </row>
-    <row r="17" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" s="1" customFormat="1">
       <c r="A17" s="3" t="s">
         <v>185</v>
       </c>
@@ -1844,11 +2044,13 @@
       <c r="C17" t="s">
         <v>190</v>
       </c>
-      <c r="D17"/>
+      <c r="D17" t="s">
+        <v>190</v>
+      </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="1:6" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" s="1" customFormat="1" ht="28">
       <c r="A18" s="3" t="s">
         <v>23</v>
       </c>
@@ -1858,11 +2060,13 @@
       <c r="C18" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="D18" s="3"/>
+      <c r="D18" s="5" t="s">
+        <v>211</v>
+      </c>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
     </row>
-    <row r="19" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" s="1" customFormat="1" ht="15">
       <c r="A19" s="3" t="s">
         <v>25</v>
       </c>
@@ -1872,11 +2076,13 @@
       <c r="C19" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="D19" s="3"/>
+      <c r="D19" s="5" t="s">
+        <v>214</v>
+      </c>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
     </row>
-    <row r="20" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" s="1" customFormat="1">
       <c r="A20" s="3" t="s">
         <v>26</v>
       </c>
@@ -1888,7 +2094,7 @@
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" s="1" customFormat="1">
       <c r="A21" s="3" t="s">
         <v>27</v>
       </c>
@@ -1900,7 +2106,7 @@
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
     </row>
-    <row r="22" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" s="1" customFormat="1" ht="28">
       <c r="A22" s="3" t="s">
         <v>28</v>
       </c>
@@ -1912,7 +2118,7 @@
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
     </row>
-    <row r="23" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" s="1" customFormat="1" ht="15">
       <c r="A23" s="3" t="s">
         <v>29</v>
       </c>
@@ -1922,11 +2128,13 @@
       <c r="C23" t="s">
         <v>189</v>
       </c>
-      <c r="D23"/>
+      <c r="D23" s="5" t="s">
+        <v>210</v>
+      </c>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
     </row>
-    <row r="24" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" s="1" customFormat="1" ht="15">
       <c r="A24" s="3" t="s">
         <v>35</v>
       </c>
@@ -1936,11 +2144,13 @@
       <c r="C24" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="D24" s="3"/>
+      <c r="D24" s="5" t="s">
+        <v>215</v>
+      </c>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
     </row>
-    <row r="25" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" s="1" customFormat="1" ht="15">
       <c r="A25" s="3" t="s">
         <v>37</v>
       </c>
@@ -1950,11 +2160,13 @@
       <c r="C25" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="D25" s="3"/>
+      <c r="D25" s="5" t="s">
+        <v>215</v>
+      </c>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
     </row>
-    <row r="26" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" s="1" customFormat="1" ht="15">
       <c r="A26" s="3" t="s">
         <v>39</v>
       </c>
@@ -1964,11 +2176,13 @@
       <c r="C26" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="D26" s="3"/>
+      <c r="D26" s="5" t="s">
+        <v>216</v>
+      </c>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
     </row>
-    <row r="27" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" s="1" customFormat="1" ht="28">
       <c r="A27" s="3" t="s">
         <v>40</v>
       </c>
@@ -1978,11 +2192,13 @@
       <c r="C27" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="D27" s="3"/>
+      <c r="D27" s="5" t="s">
+        <v>216</v>
+      </c>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
     </row>
-    <row r="28" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" s="1" customFormat="1" ht="15">
       <c r="A28" s="3" t="s">
         <v>43</v>
       </c>
@@ -1992,11 +2208,13 @@
       <c r="C28" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="D28" s="3"/>
+      <c r="D28" s="5" t="s">
+        <v>217</v>
+      </c>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
     </row>
-    <row r="29" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" s="1" customFormat="1" ht="15">
       <c r="A29" s="3" t="s">
         <v>45</v>
       </c>
@@ -2006,11 +2224,13 @@
       <c r="C29" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="D29" s="3"/>
+      <c r="D29" s="5" t="s">
+        <v>217</v>
+      </c>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
     </row>
-    <row r="30" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" s="1" customFormat="1" ht="15">
       <c r="A30" s="3" t="s">
         <v>46</v>
       </c>
@@ -2020,11 +2240,13 @@
       <c r="C30" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="D30" s="3"/>
+      <c r="D30" s="5" t="s">
+        <v>217</v>
+      </c>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
     </row>
-    <row r="31" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" s="1" customFormat="1" ht="15">
       <c r="A31" s="3" t="s">
         <v>47</v>
       </c>
@@ -2034,11 +2256,13 @@
       <c r="C31" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="D31" s="3"/>
+      <c r="D31" s="5" t="s">
+        <v>217</v>
+      </c>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
     </row>
-    <row r="32" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" s="1" customFormat="1" ht="15">
       <c r="A32" s="3" t="s">
         <v>48</v>
       </c>
@@ -2048,11 +2272,13 @@
       <c r="C32" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="D32" s="3"/>
+      <c r="D32" s="5" t="s">
+        <v>217</v>
+      </c>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
     </row>
-    <row r="33" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" s="1" customFormat="1" ht="15">
       <c r="A33" s="3" t="s">
         <v>53</v>
       </c>
@@ -2062,11 +2288,13 @@
       <c r="C33" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="D33" s="3"/>
+      <c r="D33" s="5" t="s">
+        <v>210</v>
+      </c>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
     </row>
-    <row r="34" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" s="1" customFormat="1" ht="15">
       <c r="A34" s="3" t="s">
         <v>54</v>
       </c>
@@ -2076,11 +2304,13 @@
       <c r="C34" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="D34" s="3"/>
+      <c r="D34" s="5" t="s">
+        <v>218</v>
+      </c>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
     </row>
-    <row r="35" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" s="1" customFormat="1">
       <c r="A35" s="3" t="s">
         <v>55</v>
       </c>
@@ -2092,19 +2322,23 @@
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
     </row>
-    <row r="36" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" s="1" customFormat="1" ht="28">
       <c r="A36" s="3" t="s">
         <v>61</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
+      <c r="C36" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>214</v>
+      </c>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
     </row>
-    <row r="37" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" s="1" customFormat="1">
       <c r="A37" s="3" t="s">
         <v>62</v>
       </c>
@@ -2116,127 +2350,167 @@
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
     </row>
-    <row r="38" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" s="1" customFormat="1" ht="15">
       <c r="A38" s="3" t="s">
         <v>63</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
+      <c r="C38" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>220</v>
+      </c>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
     </row>
-    <row r="39" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" s="1" customFormat="1" ht="15">
       <c r="A39" s="3" t="s">
         <v>65</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
+      <c r="C39" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>219</v>
+      </c>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
     </row>
-    <row r="40" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" s="1" customFormat="1" ht="28">
       <c r="A40" s="3" t="s">
         <v>66</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
+      <c r="C40" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>219</v>
+      </c>
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
     </row>
-    <row r="41" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" s="1" customFormat="1" ht="15">
       <c r="A41" s="3" t="s">
         <v>67</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
+      <c r="C41" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>220</v>
+      </c>
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
     </row>
-    <row r="42" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" s="1" customFormat="1" ht="15">
       <c r="A42" s="3" t="s">
         <v>68</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
+      <c r="C42" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>219</v>
+      </c>
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
     </row>
-    <row r="43" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" s="1" customFormat="1" ht="15">
       <c r="A43" s="3" t="s">
         <v>69</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
+      <c r="C43" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>221</v>
+      </c>
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
     </row>
-    <row r="44" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" s="1" customFormat="1" ht="15">
       <c r="A44" s="3" t="s">
         <v>70</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
+      <c r="C44" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>221</v>
+      </c>
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
     </row>
-    <row r="45" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" s="1" customFormat="1" ht="15">
       <c r="A45" s="3" t="s">
         <v>78</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
+      <c r="C45" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>222</v>
+      </c>
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
     </row>
-    <row r="46" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" s="1" customFormat="1" ht="15">
       <c r="A46" s="3" t="s">
         <v>80</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
+      <c r="C46" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>222</v>
+      </c>
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
     </row>
-    <row r="47" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" s="1" customFormat="1" ht="15">
       <c r="A47" s="3" t="s">
         <v>82</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
+      <c r="C47" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>223</v>
+      </c>
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
     </row>
-    <row r="48" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" s="1" customFormat="1">
       <c r="A48" s="3" t="s">
         <v>83</v>
       </c>
@@ -2248,7 +2522,7 @@
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
     </row>
-    <row r="49" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" s="1" customFormat="1">
       <c r="A49" s="3" t="s">
         <v>85</v>
       </c>
@@ -2260,539 +2534,720 @@
       <c r="E49" s="3"/>
       <c r="F49" s="3"/>
     </row>
-    <row r="50" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" s="1" customFormat="1" ht="15">
       <c r="A50" s="3" t="s">
         <v>87</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
+      <c r="C50" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>223</v>
+      </c>
       <c r="E50" s="3"/>
       <c r="F50" s="3"/>
     </row>
-    <row r="51" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" s="1" customFormat="1" ht="15">
       <c r="A51" s="3" t="s">
         <v>88</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
+      <c r="C51" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>223</v>
+      </c>
       <c r="E51" s="3"/>
       <c r="F51" s="3"/>
     </row>
-    <row r="52" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" s="1" customFormat="1" ht="15">
       <c r="A52" s="3" t="s">
         <v>89</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="C52" s="3"/>
-      <c r="D52" s="3"/>
+      <c r="C52" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>223</v>
+      </c>
       <c r="E52" s="3"/>
       <c r="F52" s="3"/>
     </row>
-    <row r="53" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" s="1" customFormat="1" ht="15">
       <c r="A53" s="3" t="s">
         <v>94</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C53" s="3"/>
-      <c r="D53" s="3"/>
+      <c r="C53" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>224</v>
+      </c>
       <c r="E53" s="3"/>
       <c r="F53" s="3"/>
     </row>
-    <row r="54" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" s="1" customFormat="1" ht="15">
       <c r="A54" s="3" t="s">
         <v>96</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="C54" s="3"/>
-      <c r="D54" s="3"/>
+      <c r="C54" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>224</v>
+      </c>
       <c r="E54" s="3"/>
       <c r="F54" s="3"/>
     </row>
-    <row r="55" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" s="1" customFormat="1" ht="15">
       <c r="A55" s="3" t="s">
         <v>100</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="C55" s="3"/>
-      <c r="D55" s="3"/>
+      <c r="C55" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>224</v>
+      </c>
       <c r="E55" s="3"/>
       <c r="F55" s="3"/>
     </row>
-    <row r="56" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" s="1" customFormat="1" ht="15">
       <c r="A56" s="3" t="s">
         <v>97</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="C56" s="3"/>
-      <c r="D56" s="3"/>
+      <c r="C56" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>224</v>
+      </c>
       <c r="E56" s="3"/>
       <c r="F56" s="3"/>
     </row>
-    <row r="57" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" s="1" customFormat="1" ht="15">
       <c r="A57" s="3" t="s">
         <v>98</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="C57" s="3"/>
-      <c r="D57" s="3"/>
+      <c r="C57" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>224</v>
+      </c>
       <c r="E57" s="3"/>
       <c r="F57" s="3"/>
     </row>
-    <row r="58" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" s="1" customFormat="1" ht="15">
       <c r="A58" s="3" t="s">
         <v>99</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="C58" s="3"/>
-      <c r="D58" s="3"/>
+      <c r="C58" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>224</v>
+      </c>
       <c r="E58" s="3"/>
       <c r="F58" s="3"/>
     </row>
-    <row r="59" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" s="1" customFormat="1" ht="15">
       <c r="A59" s="3" t="s">
         <v>106</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="C59" s="3"/>
-      <c r="D59" s="3"/>
+      <c r="C59" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>214</v>
+      </c>
       <c r="E59" s="3"/>
       <c r="F59" s="3"/>
     </row>
-    <row r="60" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" s="1" customFormat="1" ht="15">
       <c r="A60" s="3" t="s">
         <v>108</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="C60" s="3"/>
-      <c r="D60" s="3"/>
+      <c r="C60" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>214</v>
+      </c>
       <c r="E60" s="3"/>
       <c r="F60" s="3"/>
     </row>
-    <row r="61" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" s="1" customFormat="1" ht="28">
       <c r="A61" s="3" t="s">
         <v>113</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="C61" s="3"/>
-      <c r="D61" s="3"/>
+      <c r="C61" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>214</v>
+      </c>
       <c r="E61" s="3"/>
       <c r="F61" s="3"/>
     </row>
-    <row r="62" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" s="1" customFormat="1" ht="28">
       <c r="A62" s="3" t="s">
         <v>114</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="C62" s="3"/>
-      <c r="D62" s="3"/>
+      <c r="C62" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>214</v>
+      </c>
       <c r="E62" s="3"/>
       <c r="F62" s="3"/>
     </row>
-    <row r="63" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" s="1" customFormat="1" ht="15">
       <c r="A63" s="3" t="s">
         <v>109</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C63" s="3"/>
-      <c r="D63" s="3"/>
+      <c r="C63" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>213</v>
+      </c>
       <c r="E63" s="3"/>
       <c r="F63" s="3"/>
     </row>
-    <row r="64" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" s="1" customFormat="1" ht="15">
       <c r="A64" s="3" t="s">
         <v>110</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="C64" s="3"/>
-      <c r="D64" s="3"/>
+      <c r="C64" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>214</v>
+      </c>
       <c r="E64" s="3"/>
       <c r="F64" s="3"/>
     </row>
-    <row r="65" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" s="1" customFormat="1" ht="15">
       <c r="A65" s="3" t="s">
         <v>111</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="C65" s="3"/>
-      <c r="D65" s="3"/>
+      <c r="C65" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="D65" s="5" t="s">
+        <v>214</v>
+      </c>
       <c r="E65" s="3"/>
       <c r="F65" s="3"/>
     </row>
-    <row r="66" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" s="1" customFormat="1" ht="15">
       <c r="A66" s="3" t="s">
         <v>112</v>
       </c>
       <c r="B66" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="C66" s="3"/>
-      <c r="D66" s="3"/>
+      <c r="C66" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="D66" s="5" t="s">
+        <v>214</v>
+      </c>
       <c r="E66" s="3"/>
       <c r="F66" s="3"/>
     </row>
-    <row r="67" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" s="1" customFormat="1" ht="15">
       <c r="A67" s="3" t="s">
         <v>121</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="C67" s="3"/>
-      <c r="D67" s="3"/>
+      <c r="C67" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="D67" s="5" t="s">
+        <v>225</v>
+      </c>
       <c r="E67" s="3"/>
       <c r="F67" s="3"/>
     </row>
-    <row r="68" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" s="1" customFormat="1" ht="15">
       <c r="A68" s="3" t="s">
         <v>122</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="C68" s="3"/>
-      <c r="D68" s="3"/>
+      <c r="C68" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="D68" s="5" t="s">
+        <v>225</v>
+      </c>
       <c r="E68" s="3"/>
       <c r="F68" s="3"/>
     </row>
-    <row r="69" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" s="1" customFormat="1" ht="15">
       <c r="A69" s="3" t="s">
         <v>123</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="C69" s="3"/>
-      <c r="D69" s="3"/>
+      <c r="C69" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="D69" s="5" t="s">
+        <v>225</v>
+      </c>
       <c r="E69" s="3"/>
       <c r="F69" s="3"/>
     </row>
-    <row r="70" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" s="1" customFormat="1" ht="28">
       <c r="A70" s="3" t="s">
         <v>137</v>
       </c>
       <c r="B70" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="C70" s="3"/>
-      <c r="D70" s="3"/>
+      <c r="C70" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="D70" s="5" t="s">
+        <v>225</v>
+      </c>
       <c r="E70" s="3"/>
       <c r="F70" s="3"/>
     </row>
-    <row r="71" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" s="1" customFormat="1" ht="15">
       <c r="A71" s="3" t="s">
         <v>124</v>
       </c>
       <c r="B71" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="C71" s="3"/>
-      <c r="D71" s="3"/>
+      <c r="C71" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="D71" s="5" t="s">
+        <v>225</v>
+      </c>
       <c r="E71" s="3"/>
       <c r="F71" s="3"/>
     </row>
-    <row r="72" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" s="1" customFormat="1" ht="28">
       <c r="A72" s="3" t="s">
         <v>138</v>
       </c>
       <c r="B72" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="C72" s="3"/>
-      <c r="D72" s="3"/>
+      <c r="C72" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="D72" s="5" t="s">
+        <v>225</v>
+      </c>
       <c r="E72" s="3"/>
       <c r="F72" s="3"/>
     </row>
-    <row r="73" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" s="1" customFormat="1" ht="15">
       <c r="A73" s="3" t="s">
         <v>139</v>
       </c>
       <c r="B73" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="C73" s="3"/>
-      <c r="D73" s="3"/>
+      <c r="C73" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="D73" s="5" t="s">
+        <v>225</v>
+      </c>
       <c r="E73" s="3"/>
       <c r="F73" s="3"/>
     </row>
-    <row r="74" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" s="1" customFormat="1" ht="15">
       <c r="A74" s="3" t="s">
         <v>140</v>
       </c>
       <c r="B74" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="C74" s="3"/>
-      <c r="D74" s="3"/>
+      <c r="C74" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="D74" s="5" t="s">
+        <v>225</v>
+      </c>
       <c r="E74" s="3"/>
       <c r="F74" s="3"/>
     </row>
-    <row r="75" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" s="1" customFormat="1" ht="15">
       <c r="A75" s="3" t="s">
         <v>125</v>
       </c>
       <c r="B75" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="C75" s="3"/>
-      <c r="D75" s="3"/>
+      <c r="C75" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="D75" s="5" t="s">
+        <v>225</v>
+      </c>
       <c r="E75" s="3"/>
       <c r="F75" s="3"/>
     </row>
-    <row r="76" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" s="1" customFormat="1" ht="15">
       <c r="A76" s="3" t="s">
         <v>126</v>
       </c>
       <c r="B76" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="C76" s="3"/>
-      <c r="D76" s="3"/>
+      <c r="C76" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="D76" s="5" t="s">
+        <v>225</v>
+      </c>
       <c r="E76" s="3"/>
       <c r="F76" s="3"/>
     </row>
-    <row r="77" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" s="1" customFormat="1" ht="15">
       <c r="A77" s="3" t="s">
         <v>127</v>
       </c>
       <c r="B77" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="C77" s="3"/>
-      <c r="D77" s="3"/>
+      <c r="C77" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="D77" s="5" t="s">
+        <v>225</v>
+      </c>
       <c r="E77" s="3"/>
       <c r="F77" s="3"/>
     </row>
-    <row r="78" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" s="1" customFormat="1" ht="15">
       <c r="A78" s="3" t="s">
         <v>128</v>
       </c>
       <c r="B78" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="C78" s="3"/>
-      <c r="D78" s="3"/>
+      <c r="C78" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="D78" s="5" t="s">
+        <v>225</v>
+      </c>
       <c r="E78" s="3"/>
       <c r="F78" s="3"/>
     </row>
-    <row r="79" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" s="1" customFormat="1" ht="15">
       <c r="A79" s="3" t="s">
         <v>129</v>
       </c>
       <c r="B79" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="C79" s="3"/>
-      <c r="D79" s="3"/>
+      <c r="C79" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="D79" s="5" t="s">
+        <v>225</v>
+      </c>
       <c r="E79" s="3"/>
       <c r="F79" s="3"/>
     </row>
-    <row r="80" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" s="1" customFormat="1" ht="15">
       <c r="A80" s="3" t="s">
         <v>130</v>
       </c>
       <c r="B80" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="C80" s="3"/>
-      <c r="D80" s="3"/>
+      <c r="C80" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="D80" s="5" t="s">
+        <v>225</v>
+      </c>
       <c r="E80" s="3"/>
       <c r="F80" s="3"/>
     </row>
-    <row r="81" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" s="1" customFormat="1" ht="15">
       <c r="A81" s="3" t="s">
         <v>131</v>
       </c>
       <c r="B81" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C81" s="3"/>
-      <c r="D81" s="3"/>
+      <c r="C81" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="D81" s="5" t="s">
+        <v>225</v>
+      </c>
       <c r="E81" s="3"/>
       <c r="F81" s="3"/>
     </row>
-    <row r="82" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" s="1" customFormat="1" ht="15">
       <c r="A82" s="3" t="s">
         <v>132</v>
       </c>
       <c r="B82" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="C82" s="3"/>
-      <c r="D82" s="3"/>
+      <c r="C82" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="D82" s="5" t="s">
+        <v>225</v>
+      </c>
       <c r="E82" s="3"/>
       <c r="F82" s="3"/>
     </row>
-    <row r="83" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" s="1" customFormat="1" ht="15">
       <c r="A83" s="3" t="s">
         <v>133</v>
       </c>
       <c r="B83" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="C83" s="3"/>
-      <c r="D83" s="3"/>
+      <c r="C83" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="D83" s="5" t="s">
+        <v>225</v>
+      </c>
       <c r="E83" s="3"/>
       <c r="F83" s="3"/>
     </row>
-    <row r="84" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" s="1" customFormat="1" ht="15">
       <c r="A84" s="3" t="s">
         <v>134</v>
       </c>
       <c r="B84" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="C84" s="3"/>
-      <c r="D84" s="3"/>
+      <c r="C84" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="D84" s="5" t="s">
+        <v>225</v>
+      </c>
       <c r="E84" s="3"/>
       <c r="F84" s="3"/>
     </row>
-    <row r="85" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" s="1" customFormat="1" ht="15">
       <c r="A85" s="3" t="s">
         <v>135</v>
       </c>
       <c r="B85" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="C85" s="3"/>
-      <c r="D85" s="3"/>
+      <c r="C85" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="D85" s="5" t="s">
+        <v>225</v>
+      </c>
       <c r="E85" s="3"/>
       <c r="F85" s="3"/>
     </row>
-    <row r="86" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" s="1" customFormat="1" ht="15">
       <c r="A86" s="3" t="s">
         <v>136</v>
       </c>
       <c r="B86" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="C86" s="3"/>
-      <c r="D86" s="3"/>
+      <c r="C86" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="D86" s="5" t="s">
+        <v>225</v>
+      </c>
       <c r="E86" s="3"/>
       <c r="F86" s="3"/>
     </row>
-    <row r="87" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" s="1" customFormat="1" ht="15">
       <c r="A87" s="3" t="s">
         <v>161</v>
       </c>
       <c r="B87" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="C87" s="3"/>
-      <c r="D87" s="3"/>
+      <c r="C87" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="D87" s="5" t="s">
+        <v>226</v>
+      </c>
       <c r="E87" s="3"/>
       <c r="F87" s="3"/>
     </row>
-    <row r="88" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" s="1" customFormat="1" ht="15">
       <c r="A88" s="3" t="s">
         <v>162</v>
       </c>
       <c r="B88" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="C88" s="3"/>
-      <c r="D88" s="3"/>
+      <c r="C88" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="D88" s="5" t="s">
+        <v>227</v>
+      </c>
       <c r="E88" s="3"/>
       <c r="F88" s="3"/>
     </row>
-    <row r="89" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" s="1" customFormat="1" ht="15">
       <c r="A89" s="3" t="s">
         <v>163</v>
       </c>
       <c r="B89" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="C89" s="3"/>
-      <c r="D89" s="3"/>
+      <c r="C89" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="D89" s="5" t="s">
+        <v>228</v>
+      </c>
       <c r="E89" s="3"/>
       <c r="F89" s="3"/>
     </row>
-    <row r="90" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" s="1" customFormat="1" ht="15">
       <c r="A90" s="3" t="s">
         <v>164</v>
       </c>
       <c r="B90" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="C90" s="3"/>
-      <c r="D90" s="3"/>
+      <c r="C90" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="D90" s="5" t="s">
+        <v>221</v>
+      </c>
       <c r="E90" s="3"/>
       <c r="F90" s="3"/>
     </row>
-    <row r="91" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" s="1" customFormat="1" ht="15">
       <c r="A91" s="3" t="s">
         <v>165</v>
       </c>
       <c r="B91" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="C91" s="3"/>
-      <c r="D91" s="3"/>
+      <c r="C91" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="D91" s="5" t="s">
+        <v>221</v>
+      </c>
       <c r="E91" s="3"/>
       <c r="F91" s="3"/>
     </row>
-    <row r="92" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" s="1" customFormat="1" ht="15">
       <c r="A92" s="3" t="s">
         <v>166</v>
       </c>
       <c r="B92" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="C92" s="3"/>
-      <c r="D92" s="3"/>
+      <c r="C92" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="D92" s="5" t="s">
+        <v>221</v>
+      </c>
       <c r="E92" s="3"/>
       <c r="F92" s="3"/>
     </row>
-    <row r="93" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" s="1" customFormat="1" ht="15">
       <c r="A93" s="3" t="s">
         <v>167</v>
       </c>
       <c r="B93" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="C93" s="3"/>
-      <c r="D93" s="3"/>
+      <c r="C93" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="D93" s="5" t="s">
+        <v>221</v>
+      </c>
       <c r="E93" s="3"/>
       <c r="F93" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added most of the design items to the traceability matrix
</commit_message>
<xml_diff>
--- a/TraceabilityMatrix.xlsx
+++ b/TraceabilityMatrix.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26423"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rwilkins\Documents\GitHub\med656\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="10780" yWindow="0" windowWidth="20600" windowHeight="14240"/>
+    <workbookView xWindow="10785" yWindow="0" windowWidth="20595" windowHeight="14235"/>
   </bookViews>
   <sheets>
     <sheet name="TraceabilityMatrix" sheetId="1" r:id="rId1"/>
@@ -27,10 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="229">
-  <si>
-    <t>software design plan item</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="246">
   <si>
     <t>requirement index</t>
   </si>
@@ -714,6 +716,60 @@
   </si>
   <si>
     <t>Network Connection Test</t>
+  </si>
+  <si>
+    <t>software design index</t>
+  </si>
+  <si>
+    <t>software design title</t>
+  </si>
+  <si>
+    <t>AccountController</t>
+  </si>
+  <si>
+    <t>3.2.1.5</t>
+  </si>
+  <si>
+    <t>3.1.1.8</t>
+  </si>
+  <si>
+    <t>PatientController</t>
+  </si>
+  <si>
+    <t>3.2.1.6</t>
+  </si>
+  <si>
+    <t>Physician</t>
+  </si>
+  <si>
+    <t>PhysicianController</t>
+  </si>
+  <si>
+    <t>3.2.1.7</t>
+  </si>
+  <si>
+    <t>ExperimentAdministrator</t>
+  </si>
+  <si>
+    <t>3.2.1.4</t>
+  </si>
+  <si>
+    <t>AspNetUser</t>
+  </si>
+  <si>
+    <t>AdminEditController</t>
+  </si>
+  <si>
+    <t>AdminHomeController</t>
+  </si>
+  <si>
+    <t>SelectDataController</t>
+  </si>
+  <si>
+    <t>SelectActivityController</t>
+  </si>
+  <si>
+    <t>ExperimentController</t>
   </si>
 </sst>
 </file>
@@ -1333,7 +1389,25 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="9">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1491,15 +1565,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F93" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:F93"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="requirement index" dataDxfId="5"/>
-    <tableColumn id="2" name="requirement description" dataDxfId="4"/>
-    <tableColumn id="3" name="test plan index" dataDxfId="3"/>
-    <tableColumn id="4" name="test plan title" dataDxfId="2"/>
-    <tableColumn id="5" name="test plan description" dataDxfId="1"/>
-    <tableColumn id="6" name="software design plan item" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G93" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="A1:G93"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="requirement index" dataDxfId="6"/>
+    <tableColumn id="2" name="requirement description" dataDxfId="5"/>
+    <tableColumn id="3" name="test plan index" dataDxfId="4"/>
+    <tableColumn id="4" name="test plan title" dataDxfId="3"/>
+    <tableColumn id="5" name="test plan description" dataDxfId="2"/>
+    <tableColumn id="7" name="software design index" dataDxfId="0"/>
+    <tableColumn id="6" name="software design title" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1760,7 +1835,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1768,1475 +1843,1886 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F93"/>
+  <dimension ref="A1:G93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.83203125" customWidth="1"/>
-    <col min="2" max="2" width="85.33203125" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" customWidth="1"/>
-    <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="5" max="5" width="21.33203125" customWidth="1"/>
-    <col min="6" max="6" width="26.1640625" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" customWidth="1"/>
+    <col min="2" max="2" width="87.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" customWidth="1"/>
+    <col min="4" max="4" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.28515625" customWidth="1"/>
+    <col min="6" max="6" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C2" t="s">
+        <v>188</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="F2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>176</v>
+      </c>
+      <c r="B3" t="s">
+        <v>178</v>
+      </c>
+      <c r="C3" t="s">
+        <v>188</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="F3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>179</v>
+      </c>
+      <c r="B4" t="s">
+        <v>177</v>
+      </c>
+      <c r="C4" t="s">
+        <v>189</v>
+      </c>
+      <c r="D4" t="s">
+        <v>189</v>
+      </c>
+      <c r="F4" t="s">
+        <v>189</v>
+      </c>
+      <c r="G4" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="B5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
         <v>188</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15">
-      <c r="A2" t="s">
-        <v>175</v>
-      </c>
-      <c r="B2" t="s">
-        <v>176</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D7" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="C8" t="s">
         <v>189</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D8" t="s">
+        <v>189</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="15">
-      <c r="A3" t="s">
-        <v>177</v>
-      </c>
-      <c r="B3" t="s">
-        <v>179</v>
-      </c>
-      <c r="C3" t="s">
-        <v>189</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
-        <v>180</v>
-      </c>
-      <c r="B4" t="s">
-        <v>178</v>
-      </c>
-      <c r="C4" t="s">
-        <v>190</v>
-      </c>
-      <c r="D4" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" s="1" customFormat="1" ht="28">
-      <c r="A5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-    </row>
-    <row r="6" spans="1:6" s="1" customFormat="1" ht="15">
-      <c r="A6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="3" t="s">
+      <c r="E9" s="3"/>
+      <c r="F9" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D10" s="5" t="s">
         <v>212</v>
-      </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-    </row>
-    <row r="7" spans="1:6" s="1" customFormat="1" ht="15">
-      <c r="A7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" t="s">
-        <v>189</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-    </row>
-    <row r="8" spans="1:6" s="1" customFormat="1">
-      <c r="A8" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="C8" t="s">
-        <v>190</v>
-      </c>
-      <c r="D8" t="s">
-        <v>190</v>
-      </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-    </row>
-    <row r="9" spans="1:6" s="1" customFormat="1" ht="28">
-      <c r="A9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-    </row>
-    <row r="10" spans="1:6" s="1" customFormat="1" ht="28">
-      <c r="A10" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>213</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
-    </row>
-    <row r="11" spans="1:6" s="1" customFormat="1">
+      <c r="G10" s="3"/>
+    </row>
+    <row r="11" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-    </row>
-    <row r="12" spans="1:6" s="1" customFormat="1" ht="15">
+      <c r="F11" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" t="s">
+        <v>188</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B13" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
+        <v>188</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" t="s">
+        <v>188</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="C15" t="s">
         <v>189</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D15" t="s">
+        <v>189</v>
+      </c>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-    </row>
-    <row r="13" spans="1:6" s="1" customFormat="1" ht="15">
-      <c r="A13" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="E16" s="3"/>
+      <c r="F16" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="C17" t="s">
         <v>189</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D17" t="s">
+        <v>189</v>
+      </c>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="D18" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-    </row>
-    <row r="14" spans="1:6" s="1" customFormat="1" ht="15">
-      <c r="A14" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" t="s">
-        <v>189</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-    </row>
-    <row r="15" spans="1:6" s="1" customFormat="1">
-      <c r="A15" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="C15" t="s">
-        <v>190</v>
-      </c>
-      <c r="D15" t="s">
-        <v>190</v>
-      </c>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-    </row>
-    <row r="16" spans="1:6" s="1" customFormat="1" ht="28">
-      <c r="A16" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-    </row>
-    <row r="17" spans="1:6" s="1" customFormat="1">
-      <c r="A17" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="C17" t="s">
-        <v>190</v>
-      </c>
-      <c r="D17" t="s">
-        <v>190</v>
-      </c>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-    </row>
-    <row r="18" spans="1:6" s="1" customFormat="1" ht="28">
-      <c r="A18" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18" s="3" t="s">
+      <c r="E18" s="3"/>
+      <c r="F18" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-    </row>
-    <row r="19" spans="1:6" s="1" customFormat="1" ht="15">
-      <c r="A19" s="3" t="s">
+      <c r="B19" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B20" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-    </row>
-    <row r="20" spans="1:6" s="1" customFormat="1">
-      <c r="A20" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>31</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
-    </row>
-    <row r="21" spans="1:6" s="1" customFormat="1">
+      <c r="G20" s="3"/>
+    </row>
+    <row r="21" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
-    </row>
-    <row r="22" spans="1:6" s="1" customFormat="1" ht="28">
+      <c r="G21" s="3"/>
+    </row>
+    <row r="22" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
-    </row>
-    <row r="23" spans="1:6" s="1" customFormat="1" ht="15">
+      <c r="G22" s="3"/>
+    </row>
+    <row r="23" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C23" t="s">
-        <v>189</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>210</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="C23"/>
+      <c r="D23" s="5"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
-    </row>
-    <row r="24" spans="1:6" s="1" customFormat="1" ht="15">
+      <c r="G23" s="3"/>
+    </row>
+    <row r="24" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="C24" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-    </row>
-    <row r="25" spans="1:6" s="1" customFormat="1" ht="15">
-      <c r="A25" s="3" t="s">
+      <c r="B25" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="C25" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
-    </row>
-    <row r="26" spans="1:6" s="1" customFormat="1" ht="15">
+      <c r="G25" s="3"/>
+    </row>
+    <row r="26" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B27" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C27" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D28" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-    </row>
-    <row r="27" spans="1:6" s="1" customFormat="1" ht="28">
-      <c r="A27" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C27" s="3" t="s">
+      <c r="E28" s="3"/>
+      <c r="F28" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C29" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D29" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-    </row>
-    <row r="28" spans="1:6" s="1" customFormat="1" ht="15">
-      <c r="A28" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C28" s="3" t="s">
+      <c r="E29" s="3"/>
+      <c r="F29" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C34" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D34" s="5" t="s">
         <v>217</v>
-      </c>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-    </row>
-    <row r="29" spans="1:6" s="1" customFormat="1" ht="15">
-      <c r="A29" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-    </row>
-    <row r="30" spans="1:6" s="1" customFormat="1" ht="15">
-      <c r="A30" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-    </row>
-    <row r="31" spans="1:6" s="1" customFormat="1" ht="15">
-      <c r="A31" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-    </row>
-    <row r="32" spans="1:6" s="1" customFormat="1" ht="15">
-      <c r="A32" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
-    </row>
-    <row r="33" spans="1:6" s="1" customFormat="1" ht="15">
-      <c r="A33" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
-    </row>
-    <row r="34" spans="1:6" s="1" customFormat="1" ht="15">
-      <c r="A34" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>218</v>
       </c>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
-    </row>
-    <row r="35" spans="1:6" s="1" customFormat="1">
+      <c r="G34" s="3"/>
+    </row>
+    <row r="35" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
-    </row>
-    <row r="36" spans="1:6" s="1" customFormat="1" ht="28">
+      <c r="F35" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B37" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
-    </row>
-    <row r="37" spans="1:6" s="1" customFormat="1">
-      <c r="A37" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>60</v>
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
-    </row>
-    <row r="38" spans="1:6" s="1" customFormat="1" ht="15">
+      <c r="F37" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="C38" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="B39" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C39" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="D38" s="5" t="s">
+      <c r="D39" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D43" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
-    </row>
-    <row r="39" spans="1:6" s="1" customFormat="1" ht="15">
-      <c r="A39" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C39" s="3" t="s">
+      <c r="E43" s="3"/>
+      <c r="F43" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="G43" s="3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C44" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="D39" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
-    </row>
-    <row r="40" spans="1:6" s="1" customFormat="1" ht="28">
-      <c r="A40" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
-    </row>
-    <row r="41" spans="1:6" s="1" customFormat="1" ht="15">
-      <c r="A41" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="D41" s="5" t="s">
+      <c r="D44" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="E41" s="3"/>
-      <c r="F41" s="3"/>
-    </row>
-    <row r="42" spans="1:6" s="1" customFormat="1" ht="15">
-      <c r="A42" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="E42" s="3"/>
-      <c r="F42" s="3"/>
-    </row>
-    <row r="43" spans="1:6" s="1" customFormat="1" ht="15">
-      <c r="A43" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C43" s="3" t="s">
+      <c r="E44" s="3"/>
+      <c r="F44" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C45" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="D43" s="5" t="s">
+      <c r="D45" s="5" t="s">
         <v>221</v>
       </c>
-      <c r="E43" s="3"/>
-      <c r="F43" s="3"/>
-    </row>
-    <row r="44" spans="1:6" s="1" customFormat="1" ht="15">
-      <c r="A44" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C44" s="3" t="s">
+      <c r="E45" s="3"/>
+      <c r="F45" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C46" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="D44" s="5" t="s">
+      <c r="D46" s="5" t="s">
         <v>221</v>
       </c>
-      <c r="E44" s="3"/>
-      <c r="F44" s="3"/>
-    </row>
-    <row r="45" spans="1:6" s="1" customFormat="1" ht="15">
-      <c r="A45" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C45" s="3" t="s">
+      <c r="E46" s="3"/>
+      <c r="F46" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C47" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="D45" s="5" t="s">
+      <c r="D47" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="E45" s="3"/>
-      <c r="F45" s="3"/>
-    </row>
-    <row r="46" spans="1:6" s="1" customFormat="1" ht="15">
-      <c r="A46" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>222</v>
-      </c>
-      <c r="E46" s="3"/>
-      <c r="F46" s="3"/>
-    </row>
-    <row r="47" spans="1:6" s="1" customFormat="1" ht="15">
-      <c r="A47" s="3" t="s">
+      <c r="E47" s="3"/>
+      <c r="F47" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B47" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="D47" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="E47" s="3"/>
-      <c r="F47" s="3"/>
-    </row>
-    <row r="48" spans="1:6" s="1" customFormat="1">
-      <c r="A48" s="3" t="s">
+      <c r="B48" s="3" t="s">
         <v>83</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>84</v>
       </c>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
-      <c r="F48" s="3"/>
-    </row>
-    <row r="49" spans="1:6" s="1" customFormat="1">
+      <c r="F48" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G48" s="3" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B49" s="3" t="s">
         <v>85</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>86</v>
       </c>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
       <c r="E49" s="3"/>
-      <c r="F49" s="3"/>
-    </row>
-    <row r="50" spans="1:6" s="1" customFormat="1" ht="15">
+      <c r="F49" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G49" s="3" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="E50" s="3"/>
+      <c r="F50" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="B51" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="C50" s="3" t="s">
+      <c r="C51" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="E51" s="3"/>
+      <c r="F51" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="E52" s="3"/>
+      <c r="F52" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G52" s="3" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C53" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="D50" s="5" t="s">
+      <c r="D53" s="5" t="s">
         <v>223</v>
-      </c>
-      <c r="E50" s="3"/>
-      <c r="F50" s="3"/>
-    </row>
-    <row r="51" spans="1:6" s="1" customFormat="1" ht="15">
-      <c r="A51" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="D51" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="E51" s="3"/>
-      <c r="F51" s="3"/>
-    </row>
-    <row r="52" spans="1:6" s="1" customFormat="1" ht="15">
-      <c r="A52" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="D52" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="E52" s="3"/>
-      <c r="F52" s="3"/>
-    </row>
-    <row r="53" spans="1:6" s="1" customFormat="1" ht="15">
-      <c r="A53" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="D53" s="5" t="s">
-        <v>224</v>
       </c>
       <c r="E53" s="3"/>
       <c r="F53" s="3"/>
-    </row>
-    <row r="54" spans="1:6" s="1" customFormat="1" ht="15">
+      <c r="G53" s="3"/>
+    </row>
+    <row r="54" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E54" s="3"/>
       <c r="F54" s="3"/>
-    </row>
-    <row r="55" spans="1:6" s="1" customFormat="1" ht="15">
+      <c r="G54" s="3"/>
+    </row>
+    <row r="55" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E55" s="3"/>
       <c r="F55" s="3"/>
-    </row>
-    <row r="56" spans="1:6" s="1" customFormat="1" ht="15">
+      <c r="G55" s="3"/>
+    </row>
+    <row r="56" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E56" s="3"/>
       <c r="F56" s="3"/>
-    </row>
-    <row r="57" spans="1:6" s="1" customFormat="1" ht="15">
+      <c r="G56" s="3"/>
+    </row>
+    <row r="57" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E57" s="3"/>
       <c r="F57" s="3"/>
-    </row>
-    <row r="58" spans="1:6" s="1" customFormat="1" ht="15">
+      <c r="G57" s="3"/>
+    </row>
+    <row r="58" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E58" s="3"/>
       <c r="F58" s="3"/>
-    </row>
-    <row r="59" spans="1:6" s="1" customFormat="1" ht="15">
+      <c r="G58" s="3"/>
+    </row>
+    <row r="59" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E59" s="3"/>
+      <c r="F59" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G59" s="3" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A60" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E60" s="3"/>
+      <c r="F60" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G60" s="3" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A61" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E61" s="3"/>
+      <c r="F61" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G61" s="3" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A62" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E62" s="3"/>
+      <c r="F62" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G62" s="3" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A63" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="E63" s="3"/>
+      <c r="F63" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G63" s="3" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A64" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E64" s="3"/>
+      <c r="F64" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G64" s="3" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A65" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="D65" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E65" s="3"/>
+      <c r="F65" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G65" s="3" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A66" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B66" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="B59" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="D59" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="E59" s="3"/>
-      <c r="F59" s="3"/>
-    </row>
-    <row r="60" spans="1:6" s="1" customFormat="1" ht="15">
-      <c r="A60" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="D60" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="E60" s="3"/>
-      <c r="F60" s="3"/>
-    </row>
-    <row r="61" spans="1:6" s="1" customFormat="1" ht="28">
-      <c r="A61" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="D61" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="E61" s="3"/>
-      <c r="F61" s="3"/>
-    </row>
-    <row r="62" spans="1:6" s="1" customFormat="1" ht="28">
-      <c r="A62" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="D62" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="E62" s="3"/>
-      <c r="F62" s="3"/>
-    </row>
-    <row r="63" spans="1:6" s="1" customFormat="1" ht="15">
-      <c r="A63" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="B63" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="C63" s="3" t="s">
+      <c r="C66" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="D63" s="5" t="s">
+      <c r="D66" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="E63" s="3"/>
-      <c r="F63" s="3"/>
-    </row>
-    <row r="64" spans="1:6" s="1" customFormat="1" ht="15">
-      <c r="A64" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="B64" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="C64" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="D64" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="E64" s="3"/>
-      <c r="F64" s="3"/>
-    </row>
-    <row r="65" spans="1:6" s="1" customFormat="1" ht="15">
-      <c r="A65" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="B65" s="3" t="s">
+      <c r="E66" s="3"/>
+      <c r="F66" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G66" s="3" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A67" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="C65" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="D65" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="E65" s="3"/>
-      <c r="F65" s="3"/>
-    </row>
-    <row r="66" spans="1:6" s="1" customFormat="1" ht="15">
-      <c r="A66" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="B66" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="C66" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="D66" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="E66" s="3"/>
-      <c r="F66" s="3"/>
-    </row>
-    <row r="67" spans="1:6" s="1" customFormat="1" ht="15">
-      <c r="A67" s="3" t="s">
+      <c r="B67" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="D67" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="E67" s="3"/>
+      <c r="F67" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G67" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A68" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="B67" s="3" t="s">
+      <c r="B68" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="C67" s="3" t="s">
+      <c r="C68" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="D68" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="E68" s="3"/>
+      <c r="F68" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G68" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A69" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="D69" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="E69" s="3"/>
+      <c r="F69" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G69" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A70" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="D70" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="E70" s="3"/>
+      <c r="F70" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G70" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A71" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="D71" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="E71" s="3"/>
+      <c r="F71" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G71" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A72" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="D72" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="E72" s="3"/>
+      <c r="F72" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G72" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A73" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="D73" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="E73" s="3"/>
+      <c r="F73" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G73" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A74" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="D74" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="E74" s="3"/>
+      <c r="F74" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G74" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A75" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="D75" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="E75" s="3"/>
+      <c r="F75" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G75" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A76" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="D76" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="E76" s="3"/>
+      <c r="F76" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G76" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A77" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="D77" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="E77" s="3"/>
+      <c r="F77" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G77" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A78" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="D78" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="E78" s="3"/>
+      <c r="F78" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G78" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A79" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="D79" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="E79" s="3"/>
+      <c r="F79" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G79" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A80" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="D80" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="E80" s="3"/>
+      <c r="F80" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G80" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A81" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="D81" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="E81" s="3"/>
+      <c r="F81" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G81" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A82" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="D82" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="E82" s="3"/>
+      <c r="F82" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G82" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A83" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="D83" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="E83" s="3"/>
+      <c r="F83" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G83" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A84" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="D84" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="E84" s="3"/>
+      <c r="F84" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G84" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A85" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="D85" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="E85" s="3"/>
+      <c r="F85" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G85" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A86" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="D86" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="E86" s="3"/>
+      <c r="F86" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G86" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A87" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="C87" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="D67" s="5" t="s">
+      <c r="D87" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="E67" s="3"/>
-      <c r="F67" s="3"/>
-    </row>
-    <row r="68" spans="1:6" s="1" customFormat="1" ht="15">
-      <c r="A68" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="C68" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="D68" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="E68" s="3"/>
-      <c r="F68" s="3"/>
-    </row>
-    <row r="69" spans="1:6" s="1" customFormat="1" ht="15">
-      <c r="A69" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="B69" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="C69" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="D69" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="E69" s="3"/>
-      <c r="F69" s="3"/>
-    </row>
-    <row r="70" spans="1:6" s="1" customFormat="1" ht="28">
-      <c r="A70" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="B70" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="C70" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="D70" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="E70" s="3"/>
-      <c r="F70" s="3"/>
-    </row>
-    <row r="71" spans="1:6" s="1" customFormat="1" ht="15">
-      <c r="A71" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="B71" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="C71" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="D71" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="E71" s="3"/>
-      <c r="F71" s="3"/>
-    </row>
-    <row r="72" spans="1:6" s="1" customFormat="1" ht="28">
-      <c r="A72" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="B72" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="C72" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="D72" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="E72" s="3"/>
-      <c r="F72" s="3"/>
-    </row>
-    <row r="73" spans="1:6" s="1" customFormat="1" ht="15">
-      <c r="A73" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="B73" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="C73" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="D73" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="E73" s="3"/>
-      <c r="F73" s="3"/>
-    </row>
-    <row r="74" spans="1:6" s="1" customFormat="1" ht="15">
-      <c r="A74" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="B74" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="C74" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="D74" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="E74" s="3"/>
-      <c r="F74" s="3"/>
-    </row>
-    <row r="75" spans="1:6" s="1" customFormat="1" ht="15">
-      <c r="A75" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="B75" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="C75" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="D75" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="E75" s="3"/>
-      <c r="F75" s="3"/>
-    </row>
-    <row r="76" spans="1:6" s="1" customFormat="1" ht="15">
-      <c r="A76" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="B76" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="C76" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="D76" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="E76" s="3"/>
-      <c r="F76" s="3"/>
-    </row>
-    <row r="77" spans="1:6" s="1" customFormat="1" ht="15">
-      <c r="A77" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="B77" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="C77" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="D77" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="E77" s="3"/>
-      <c r="F77" s="3"/>
-    </row>
-    <row r="78" spans="1:6" s="1" customFormat="1" ht="15">
-      <c r="A78" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="B78" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="C78" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="D78" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="E78" s="3"/>
-      <c r="F78" s="3"/>
-    </row>
-    <row r="79" spans="1:6" s="1" customFormat="1" ht="15">
-      <c r="A79" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="B79" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="C79" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="D79" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="E79" s="3"/>
-      <c r="F79" s="3"/>
-    </row>
-    <row r="80" spans="1:6" s="1" customFormat="1" ht="15">
-      <c r="A80" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="B80" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="C80" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="D80" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="E80" s="3"/>
-      <c r="F80" s="3"/>
-    </row>
-    <row r="81" spans="1:6" s="1" customFormat="1" ht="15">
-      <c r="A81" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="B81" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="C81" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="D81" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="E81" s="3"/>
-      <c r="F81" s="3"/>
-    </row>
-    <row r="82" spans="1:6" s="1" customFormat="1" ht="15">
-      <c r="A82" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="B82" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="C82" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="D82" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="E82" s="3"/>
-      <c r="F82" s="3"/>
-    </row>
-    <row r="83" spans="1:6" s="1" customFormat="1" ht="15">
-      <c r="A83" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="B83" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="C83" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="D83" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="E83" s="3"/>
-      <c r="F83" s="3"/>
-    </row>
-    <row r="84" spans="1:6" s="1" customFormat="1" ht="15">
-      <c r="A84" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="B84" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="C84" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="D84" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="E84" s="3"/>
-      <c r="F84" s="3"/>
-    </row>
-    <row r="85" spans="1:6" s="1" customFormat="1" ht="15">
-      <c r="A85" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="B85" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="C85" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="D85" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="E85" s="3"/>
-      <c r="F85" s="3"/>
-    </row>
-    <row r="86" spans="1:6" s="1" customFormat="1" ht="15">
-      <c r="A86" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="B86" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="C86" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="D86" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="E86" s="3"/>
-      <c r="F86" s="3"/>
-    </row>
-    <row r="87" spans="1:6" s="1" customFormat="1" ht="15">
-      <c r="A87" s="3" t="s">
+      <c r="E87" s="3"/>
+      <c r="F87" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="G87" s="3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A88" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="B87" s="3" t="s">
+      <c r="B88" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="C87" s="3" t="s">
+      <c r="C88" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="D87" s="5" t="s">
+      <c r="D88" s="5" t="s">
         <v>226</v>
       </c>
-      <c r="E87" s="3"/>
-      <c r="F87" s="3"/>
-    </row>
-    <row r="88" spans="1:6" s="1" customFormat="1" ht="15">
-      <c r="A88" s="3" t="s">
+      <c r="E88" s="3"/>
+      <c r="F88" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="G88" s="3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A89" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="B88" s="3" t="s">
+      <c r="B89" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="C88" s="3" t="s">
+      <c r="C89" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="D88" s="5" t="s">
+      <c r="D89" s="5" t="s">
         <v>227</v>
       </c>
-      <c r="E88" s="3"/>
-      <c r="F88" s="3"/>
-    </row>
-    <row r="89" spans="1:6" s="1" customFormat="1" ht="15">
-      <c r="A89" s="3" t="s">
+      <c r="E89" s="3"/>
+      <c r="F89" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="G89" s="3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A90" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="B89" s="3" t="s">
+      <c r="B90" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="C89" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="D89" s="5" t="s">
-        <v>228</v>
-      </c>
-      <c r="E89" s="3"/>
-      <c r="F89" s="3"/>
-    </row>
-    <row r="90" spans="1:6" s="1" customFormat="1" ht="15">
-      <c r="A90" s="3" t="s">
+      <c r="C90" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D90" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="E90" s="3"/>
+      <c r="F90" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G90" s="3" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A91" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="B90" s="3" t="s">
+      <c r="B91" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="C90" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="D90" s="5" t="s">
-        <v>221</v>
-      </c>
-      <c r="E90" s="3"/>
-      <c r="F90" s="3"/>
-    </row>
-    <row r="91" spans="1:6" s="1" customFormat="1" ht="15">
-      <c r="A91" s="3" t="s">
+      <c r="C91" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D91" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="E91" s="3"/>
+      <c r="F91" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G91" s="3" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A92" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="B91" s="3" t="s">
+      <c r="B92" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="C91" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="D91" s="5" t="s">
-        <v>221</v>
-      </c>
-      <c r="E91" s="3"/>
-      <c r="F91" s="3"/>
-    </row>
-    <row r="92" spans="1:6" s="1" customFormat="1" ht="15">
-      <c r="A92" s="3" t="s">
+      <c r="C92" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D92" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="E92" s="3"/>
+      <c r="F92" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G92" s="3" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A93" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="B92" s="3" t="s">
+      <c r="B93" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="C92" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="D92" s="5" t="s">
-        <v>221</v>
-      </c>
-      <c r="E92" s="3"/>
-      <c r="F92" s="3"/>
-    </row>
-    <row r="93" spans="1:6" s="1" customFormat="1" ht="15">
-      <c r="A93" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="B93" s="3" t="s">
-        <v>174</v>
-      </c>
       <c r="C93" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D93" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E93" s="3"/>
-      <c r="F93" s="3"/>
+      <c r="F93" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G93" s="3" t="s">
+        <v>244</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated the traceability matrix
</commit_message>
<xml_diff>
--- a/TraceabilityMatrix.xlsx
+++ b/TraceabilityMatrix.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26423"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rwilkins\Documents\GitHub\med656\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="10785" yWindow="0" windowWidth="20595" windowHeight="14235"/>
+    <workbookView xWindow="0" yWindow="-460" windowWidth="51200" windowHeight="28800"/>
   </bookViews>
   <sheets>
     <sheet name="TraceabilityMatrix" sheetId="1" r:id="rId1"/>
@@ -32,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="250">
   <si>
     <t>requirement index</t>
   </si>
@@ -770,6 +765,18 @@
   </si>
   <si>
     <t>ExperimentController</t>
+  </si>
+  <si>
+    <t>5.2.1.20</t>
+  </si>
+  <si>
+    <t>Graph View Tests</t>
+  </si>
+  <si>
+    <t>5.2.1.21</t>
+  </si>
+  <si>
+    <t>Patient/Physician Association Tests</t>
   </si>
 </sst>
 </file>
@@ -1247,7 +1254,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="62">
+  <cellStyleXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1310,6 +1317,10 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1325,7 +1336,7 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="62">
+  <cellStyles count="66">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1364,6 +1375,8 @@
     <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
@@ -1379,6 +1392,8 @@
     <cellStyle name="Hyperlink" xfId="56" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="62" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="64" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1573,8 +1588,8 @@
     <tableColumn id="3" name="test plan index" dataDxfId="4"/>
     <tableColumn id="4" name="test plan title" dataDxfId="3"/>
     <tableColumn id="5" name="test plan description" dataDxfId="2"/>
-    <tableColumn id="7" name="software design index" dataDxfId="0"/>
-    <tableColumn id="6" name="software design title" dataDxfId="1"/>
+    <tableColumn id="7" name="software design index" dataDxfId="1"/>
+    <tableColumn id="6" name="software design title" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1835,7 +1850,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1845,22 +1860,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" customWidth="1"/>
-    <col min="2" max="2" width="87.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" customWidth="1"/>
-    <col min="4" max="4" width="36.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.28515625" customWidth="1"/>
-    <col min="6" max="6" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.28515625" customWidth="1"/>
+    <col min="1" max="1" width="19.83203125" customWidth="1"/>
+    <col min="2" max="2" width="87.5" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" customWidth="1"/>
+    <col min="4" max="4" width="36.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.33203125" customWidth="1"/>
+    <col min="6" max="6" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1883,7 +1898,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15">
       <c r="A2" t="s">
         <v>174</v>
       </c>
@@ -1903,7 +1918,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15">
       <c r="A3" t="s">
         <v>176</v>
       </c>
@@ -1923,7 +1938,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>179</v>
       </c>
@@ -1943,7 +1958,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" s="1" customFormat="1" ht="28">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
@@ -1964,7 +1979,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" s="1" customFormat="1" ht="15">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -1985,7 +2000,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" s="1" customFormat="1" ht="15">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
@@ -2006,7 +2021,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" s="1" customFormat="1">
       <c r="A8" s="3" t="s">
         <v>180</v>
       </c>
@@ -2027,7 +2042,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" s="1" customFormat="1" ht="28">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
@@ -2048,7 +2063,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" s="1" customFormat="1" ht="28">
       <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
@@ -2062,18 +2077,26 @@
         <v>212</v>
       </c>
       <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-    </row>
-    <row r="11" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F10" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="1" customFormat="1">
       <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
+      <c r="C11" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>247</v>
+      </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3" t="s">
         <v>53</v>
@@ -2082,7 +2105,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" s="1" customFormat="1" ht="15">
       <c r="A12" s="3" t="s">
         <v>12</v>
       </c>
@@ -2103,7 +2126,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" s="1" customFormat="1" ht="15">
       <c r="A13" s="3" t="s">
         <v>13</v>
       </c>
@@ -2124,7 +2147,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" s="1" customFormat="1" ht="15">
       <c r="A14" s="3" t="s">
         <v>14</v>
       </c>
@@ -2145,7 +2168,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" s="1" customFormat="1">
       <c r="A15" s="3" t="s">
         <v>182</v>
       </c>
@@ -2166,7 +2189,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" s="1" customFormat="1" ht="28">
       <c r="A16" s="3" t="s">
         <v>20</v>
       </c>
@@ -2187,7 +2210,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" s="1" customFormat="1">
       <c r="A17" s="3" t="s">
         <v>184</v>
       </c>
@@ -2208,7 +2231,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" s="1" customFormat="1" ht="28">
       <c r="A18" s="3" t="s">
         <v>22</v>
       </c>
@@ -2229,7 +2252,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" s="1" customFormat="1" ht="15">
       <c r="A19" s="3" t="s">
         <v>24</v>
       </c>
@@ -2250,46 +2273,58 @@
         <v>241</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" s="1" customFormat="1">
       <c r="A20" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
+      <c r="C20" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>249</v>
+      </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
     </row>
-    <row r="21" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" s="1" customFormat="1">
       <c r="A21" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
+      <c r="C21" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>217</v>
+      </c>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
     </row>
-    <row r="22" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" s="1" customFormat="1" ht="28">
       <c r="A22" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
+      <c r="C22" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>212</v>
+      </c>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
     </row>
-    <row r="23" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" s="1" customFormat="1" ht="15">
       <c r="A23" s="3" t="s">
         <v>28</v>
       </c>
@@ -2302,7 +2337,7 @@
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
     </row>
-    <row r="24" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" s="1" customFormat="1" ht="15">
       <c r="A24" s="3" t="s">
         <v>34</v>
       </c>
@@ -2323,7 +2358,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="25" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" s="1" customFormat="1" ht="15">
       <c r="A25" s="3" t="s">
         <v>36</v>
       </c>
@@ -2340,7 +2375,7 @@
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
     </row>
-    <row r="26" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" s="1" customFormat="1" ht="15">
       <c r="A26" s="3" t="s">
         <v>38</v>
       </c>
@@ -2361,7 +2396,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="27" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" s="1" customFormat="1" ht="28">
       <c r="A27" s="3" t="s">
         <v>39</v>
       </c>
@@ -2382,7 +2417,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="28" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" s="1" customFormat="1" ht="15">
       <c r="A28" s="3" t="s">
         <v>42</v>
       </c>
@@ -2403,7 +2438,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="29" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" s="1" customFormat="1" ht="15">
       <c r="A29" s="3" t="s">
         <v>44</v>
       </c>
@@ -2424,7 +2459,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="30" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" s="1" customFormat="1" ht="15">
       <c r="A30" s="3" t="s">
         <v>45</v>
       </c>
@@ -2445,7 +2480,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="31" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" s="1" customFormat="1" ht="15">
       <c r="A31" s="3" t="s">
         <v>46</v>
       </c>
@@ -2466,7 +2501,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="32" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" s="1" customFormat="1" ht="15">
       <c r="A32" s="3" t="s">
         <v>47</v>
       </c>
@@ -2487,7 +2522,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="33" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" s="1" customFormat="1" ht="15">
       <c r="A33" s="3" t="s">
         <v>52</v>
       </c>
@@ -2508,7 +2543,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="34" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" s="1" customFormat="1" ht="15">
       <c r="A34" s="3" t="s">
         <v>53</v>
       </c>
@@ -2525,15 +2560,19 @@
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
     </row>
-    <row r="35" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" s="1" customFormat="1">
       <c r="A35" s="3" t="s">
         <v>54</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
+      <c r="C35" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>213</v>
+      </c>
       <c r="E35" s="3"/>
       <c r="F35" s="3" t="s">
         <v>38</v>
@@ -2542,7 +2581,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="36" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" s="1" customFormat="1" ht="28">
       <c r="A36" s="3" t="s">
         <v>60</v>
       </c>
@@ -2563,15 +2602,19 @@
         <v>242</v>
       </c>
     </row>
-    <row r="37" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" s="1" customFormat="1">
       <c r="A37" s="3" t="s">
         <v>61</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
+      <c r="C37" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>213</v>
+      </c>
       <c r="E37" s="3"/>
       <c r="F37" s="3" t="s">
         <v>53</v>
@@ -2580,7 +2623,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="38" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" s="1" customFormat="1" ht="15">
       <c r="A38" s="3" t="s">
         <v>62</v>
       </c>
@@ -2601,7 +2644,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="39" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" s="1" customFormat="1" ht="15">
       <c r="A39" s="3" t="s">
         <v>64</v>
       </c>
@@ -2622,7 +2665,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="40" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" s="1" customFormat="1" ht="28">
       <c r="A40" s="3" t="s">
         <v>65</v>
       </c>
@@ -2643,7 +2686,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="41" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" s="1" customFormat="1" ht="15">
       <c r="A41" s="3" t="s">
         <v>66</v>
       </c>
@@ -2664,7 +2707,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="42" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" s="1" customFormat="1" ht="15">
       <c r="A42" s="3" t="s">
         <v>67</v>
       </c>
@@ -2685,7 +2728,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="43" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" s="1" customFormat="1" ht="15">
       <c r="A43" s="3" t="s">
         <v>68</v>
       </c>
@@ -2706,7 +2749,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="44" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" s="1" customFormat="1" ht="15">
       <c r="A44" s="3" t="s">
         <v>69</v>
       </c>
@@ -2727,7 +2770,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="45" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" s="1" customFormat="1" ht="15">
       <c r="A45" s="3" t="s">
         <v>77</v>
       </c>
@@ -2748,7 +2791,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="46" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" s="1" customFormat="1" ht="15">
       <c r="A46" s="3" t="s">
         <v>79</v>
       </c>
@@ -2769,7 +2812,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="47" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" s="1" customFormat="1" ht="15">
       <c r="A47" s="3" t="s">
         <v>81</v>
       </c>
@@ -2790,15 +2833,19 @@
         <v>245</v>
       </c>
     </row>
-    <row r="48" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" s="1" customFormat="1" ht="15">
       <c r="A48" s="3" t="s">
         <v>82</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C48" s="3"/>
-      <c r="D48" s="3"/>
+      <c r="C48" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>222</v>
+      </c>
       <c r="E48" s="3"/>
       <c r="F48" s="3" t="s">
         <v>54</v>
@@ -2807,15 +2854,19 @@
         <v>245</v>
       </c>
     </row>
-    <row r="49" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" s="1" customFormat="1" ht="15">
       <c r="A49" s="3" t="s">
         <v>84</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
+      <c r="C49" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>222</v>
+      </c>
       <c r="E49" s="3"/>
       <c r="F49" s="3" t="s">
         <v>54</v>
@@ -2824,7 +2875,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="50" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" s="1" customFormat="1" ht="15">
       <c r="A50" s="3" t="s">
         <v>86</v>
       </c>
@@ -2845,7 +2896,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="51" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" s="1" customFormat="1" ht="15">
       <c r="A51" s="3" t="s">
         <v>87</v>
       </c>
@@ -2866,7 +2917,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="52" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" s="1" customFormat="1" ht="15">
       <c r="A52" s="3" t="s">
         <v>88</v>
       </c>
@@ -2887,7 +2938,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="53" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" s="1" customFormat="1" ht="15">
       <c r="A53" s="3" t="s">
         <v>93</v>
       </c>
@@ -2904,7 +2955,7 @@
       <c r="F53" s="3"/>
       <c r="G53" s="3"/>
     </row>
-    <row r="54" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" s="1" customFormat="1" ht="15">
       <c r="A54" s="3" t="s">
         <v>95</v>
       </c>
@@ -2921,7 +2972,7 @@
       <c r="F54" s="3"/>
       <c r="G54" s="3"/>
     </row>
-    <row r="55" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" s="1" customFormat="1" ht="15">
       <c r="A55" s="3" t="s">
         <v>99</v>
       </c>
@@ -2938,7 +2989,7 @@
       <c r="F55" s="3"/>
       <c r="G55" s="3"/>
     </row>
-    <row r="56" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" s="1" customFormat="1" ht="15">
       <c r="A56" s="3" t="s">
         <v>96</v>
       </c>
@@ -2955,7 +3006,7 @@
       <c r="F56" s="3"/>
       <c r="G56" s="3"/>
     </row>
-    <row r="57" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" s="1" customFormat="1" ht="15">
       <c r="A57" s="3" t="s">
         <v>97</v>
       </c>
@@ -2972,7 +3023,7 @@
       <c r="F57" s="3"/>
       <c r="G57" s="3"/>
     </row>
-    <row r="58" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" s="1" customFormat="1" ht="15">
       <c r="A58" s="3" t="s">
         <v>98</v>
       </c>
@@ -2989,7 +3040,7 @@
       <c r="F58" s="3"/>
       <c r="G58" s="3"/>
     </row>
-    <row r="59" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" s="1" customFormat="1" ht="15">
       <c r="A59" s="3" t="s">
         <v>105</v>
       </c>
@@ -3010,7 +3061,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="60" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" s="1" customFormat="1" ht="15">
       <c r="A60" s="3" t="s">
         <v>107</v>
       </c>
@@ -3031,7 +3082,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="61" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" s="1" customFormat="1" ht="28">
       <c r="A61" s="3" t="s">
         <v>112</v>
       </c>
@@ -3052,7 +3103,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="62" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" s="1" customFormat="1" ht="15">
       <c r="A62" s="3" t="s">
         <v>113</v>
       </c>
@@ -3073,7 +3124,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="63" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" s="1" customFormat="1" ht="15">
       <c r="A63" s="3" t="s">
         <v>108</v>
       </c>
@@ -3094,7 +3145,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="64" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" s="1" customFormat="1" ht="15">
       <c r="A64" s="3" t="s">
         <v>109</v>
       </c>
@@ -3115,7 +3166,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="65" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" s="1" customFormat="1" ht="15">
       <c r="A65" s="3" t="s">
         <v>110</v>
       </c>
@@ -3136,7 +3187,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="66" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" s="1" customFormat="1" ht="15">
       <c r="A66" s="3" t="s">
         <v>111</v>
       </c>
@@ -3157,7 +3208,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="67" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" s="1" customFormat="1" ht="15">
       <c r="A67" s="3" t="s">
         <v>120</v>
       </c>
@@ -3178,7 +3229,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="68" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" s="1" customFormat="1" ht="15">
       <c r="A68" s="3" t="s">
         <v>121</v>
       </c>
@@ -3199,7 +3250,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="69" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" s="1" customFormat="1" ht="15">
       <c r="A69" s="3" t="s">
         <v>122</v>
       </c>
@@ -3220,7 +3271,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="70" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" s="1" customFormat="1" ht="28">
       <c r="A70" s="3" t="s">
         <v>136</v>
       </c>
@@ -3241,7 +3292,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="71" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" s="1" customFormat="1" ht="15">
       <c r="A71" s="3" t="s">
         <v>123</v>
       </c>
@@ -3262,7 +3313,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="72" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" s="1" customFormat="1" ht="28">
       <c r="A72" s="3" t="s">
         <v>137</v>
       </c>
@@ -3283,7 +3334,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="73" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" s="1" customFormat="1" ht="15">
       <c r="A73" s="3" t="s">
         <v>138</v>
       </c>
@@ -3304,7 +3355,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="74" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" s="1" customFormat="1" ht="15">
       <c r="A74" s="3" t="s">
         <v>139</v>
       </c>
@@ -3325,7 +3376,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="75" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" s="1" customFormat="1" ht="15">
       <c r="A75" s="3" t="s">
         <v>124</v>
       </c>
@@ -3346,7 +3397,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="76" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" s="1" customFormat="1" ht="15">
       <c r="A76" s="3" t="s">
         <v>125</v>
       </c>
@@ -3367,7 +3418,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="77" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" s="1" customFormat="1" ht="15">
       <c r="A77" s="3" t="s">
         <v>126</v>
       </c>
@@ -3388,7 +3439,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="78" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" s="1" customFormat="1" ht="15">
       <c r="A78" s="3" t="s">
         <v>127</v>
       </c>
@@ -3409,7 +3460,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="79" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" s="1" customFormat="1" ht="15">
       <c r="A79" s="3" t="s">
         <v>128</v>
       </c>
@@ -3430,7 +3481,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="80" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" s="1" customFormat="1" ht="15">
       <c r="A80" s="3" t="s">
         <v>129</v>
       </c>
@@ -3451,7 +3502,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="81" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" s="1" customFormat="1" ht="15">
       <c r="A81" s="3" t="s">
         <v>130</v>
       </c>
@@ -3472,7 +3523,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="82" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" s="1" customFormat="1" ht="15">
       <c r="A82" s="3" t="s">
         <v>131</v>
       </c>
@@ -3493,7 +3544,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="83" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" s="1" customFormat="1" ht="15">
       <c r="A83" s="3" t="s">
         <v>132</v>
       </c>
@@ -3514,7 +3565,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="84" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" s="1" customFormat="1" ht="15">
       <c r="A84" s="3" t="s">
         <v>133</v>
       </c>
@@ -3535,7 +3586,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="85" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" s="1" customFormat="1" ht="15">
       <c r="A85" s="3" t="s">
         <v>134</v>
       </c>
@@ -3556,7 +3607,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="86" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" s="1" customFormat="1" ht="15">
       <c r="A86" s="3" t="s">
         <v>135</v>
       </c>
@@ -3577,7 +3628,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="87" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" s="1" customFormat="1" ht="15">
       <c r="A87" s="3" t="s">
         <v>160</v>
       </c>
@@ -3598,7 +3649,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="88" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" s="1" customFormat="1" ht="15">
       <c r="A88" s="3" t="s">
         <v>161</v>
       </c>
@@ -3619,7 +3670,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="89" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" s="1" customFormat="1" ht="15">
       <c r="A89" s="3" t="s">
         <v>162</v>
       </c>
@@ -3640,7 +3691,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="90" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" s="1" customFormat="1" ht="15">
       <c r="A90" s="3" t="s">
         <v>163</v>
       </c>
@@ -3661,7 +3712,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="91" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" s="1" customFormat="1" ht="15">
       <c r="A91" s="3" t="s">
         <v>164</v>
       </c>
@@ -3682,7 +3733,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="92" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" s="1" customFormat="1" ht="15">
       <c r="A92" s="3" t="s">
         <v>165</v>
       </c>
@@ -3703,7 +3754,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="93" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" s="1" customFormat="1" ht="15">
       <c r="A93" s="3" t="s">
         <v>166</v>
       </c>

</xml_diff>

<commit_message>
added columns for tracing test descriptions
</commit_message>
<xml_diff>
--- a/TraceabilityMatrix.xlsx
+++ b/TraceabilityMatrix.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rwilkins\Documents\GitHub\med656\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="-465" windowWidth="29040" windowHeight="16440"/>
   </bookViews>
@@ -27,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="297">
   <si>
     <t>requirement index</t>
   </si>
@@ -576,9 +581,6 @@
   </si>
   <si>
     <t>test plan index</t>
-  </si>
-  <si>
-    <t>test plan description</t>
   </si>
   <si>
     <t>5.2.1.1</t>
@@ -776,13 +778,160 @@
   </si>
   <si>
     <t>Physican Controller</t>
+  </si>
+  <si>
+    <t>test description index</t>
+  </si>
+  <si>
+    <t>test description title</t>
+  </si>
+  <si>
+    <t>pytest.Login</t>
+  </si>
+  <si>
+    <t>4.1.3</t>
+  </si>
+  <si>
+    <t>Create Patient</t>
+  </si>
+  <si>
+    <t>4.5.1</t>
+  </si>
+  <si>
+    <t>Patient to Patient</t>
+  </si>
+  <si>
+    <t>4.1.1</t>
+  </si>
+  <si>
+    <t>Create Physician</t>
+  </si>
+  <si>
+    <t>4.2.1</t>
+  </si>
+  <si>
+    <t>Physician can edit his account</t>
+  </si>
+  <si>
+    <t>4.5.2</t>
+  </si>
+  <si>
+    <t>Physician to patient</t>
+  </si>
+  <si>
+    <t>4.1.4</t>
+  </si>
+  <si>
+    <t>Delete patient</t>
+  </si>
+  <si>
+    <t>4.1.2</t>
+  </si>
+  <si>
+    <t>Create Experiment Admin</t>
+  </si>
+  <si>
+    <t>4.4.6</t>
+  </si>
+  <si>
+    <t>Reset Password</t>
+  </si>
+  <si>
+    <t>4.2.2</t>
+  </si>
+  <si>
+    <t>Sys Admin can edit patient account</t>
+  </si>
+  <si>
+    <t>4.7.1</t>
+  </si>
+  <si>
+    <t>Username cannot be copied</t>
+  </si>
+  <si>
+    <t>4.4.1</t>
+  </si>
+  <si>
+    <t>Good Password</t>
+  </si>
+  <si>
+    <t>4.4.2</t>
+  </si>
+  <si>
+    <t>Password Length</t>
+  </si>
+  <si>
+    <t>4.4.3</t>
+  </si>
+  <si>
+    <t>Password Case</t>
+  </si>
+  <si>
+    <t>4.4.4</t>
+  </si>
+  <si>
+    <t>Password Digit</t>
+  </si>
+  <si>
+    <t>4.4.5</t>
+  </si>
+  <si>
+    <t>Password Special Char</t>
+  </si>
+  <si>
+    <t>4.3.1</t>
+  </si>
+  <si>
+    <t>4.6.1</t>
+  </si>
+  <si>
+    <t>Login Physician</t>
+  </si>
+  <si>
+    <t>4.1.5</t>
+  </si>
+  <si>
+    <t>Pytest.Upload</t>
+  </si>
+  <si>
+    <t>4.6.2</t>
+  </si>
+  <si>
+    <t>4.6.3</t>
+  </si>
+  <si>
+    <t>Multi File No Activity</t>
+  </si>
+  <si>
+    <t>Single File One Activity</t>
+  </si>
+  <si>
+    <t>4.6.7</t>
+  </si>
+  <si>
+    <t>Zephyr Data Upload</t>
+  </si>
+  <si>
+    <t>Creat Physician</t>
+  </si>
+  <si>
+    <t>Delete Physician</t>
+  </si>
+  <si>
+    <t>Single File No Activity</t>
+  </si>
+  <si>
+    <t>4.6.8</t>
+  </si>
+  <si>
+    <t>Mband Data Upload</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -943,6 +1092,12 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="33">
@@ -1321,7 +1476,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1334,6 +1489,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="66">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1403,7 +1564,24 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1579,16 +1757,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G91" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="A1:G91"/>
-  <tableColumns count="7">
-    <tableColumn id="1" name="requirement index" dataDxfId="6"/>
-    <tableColumn id="2" name="requirement description" dataDxfId="5"/>
-    <tableColumn id="3" name="test plan index" dataDxfId="4"/>
-    <tableColumn id="4" name="test plan title" dataDxfId="3"/>
-    <tableColumn id="5" name="test plan description" dataDxfId="2"/>
-    <tableColumn id="7" name="software design index" dataDxfId="1"/>
-    <tableColumn id="6" name="software design title" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H91" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="A1:H91"/>
+  <tableColumns count="8">
+    <tableColumn id="1" name="requirement index" dataDxfId="7"/>
+    <tableColumn id="2" name="requirement description" dataDxfId="6"/>
+    <tableColumn id="3" name="test plan index" dataDxfId="5"/>
+    <tableColumn id="4" name="test plan title" dataDxfId="4"/>
+    <tableColumn id="8" name="test description index" dataDxfId="0"/>
+    <tableColumn id="5" name="test description title" dataDxfId="3"/>
+    <tableColumn id="7" name="software design index" dataDxfId="2"/>
+    <tableColumn id="6" name="software design title" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1849,7 +2028,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1857,10 +2036,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G91"/>
+  <dimension ref="A1:H91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="E92" sqref="E92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1869,12 +2048,13 @@
     <col min="2" max="2" width="87.42578125" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" customWidth="1"/>
     <col min="4" max="4" width="36.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.28515625" customWidth="1"/>
-    <col min="6" max="6" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.28515625" customWidth="1"/>
+    <col min="5" max="5" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1885,19 +2065,22 @@
         <v>182</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>183</v>
+        <v>248</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>170</v>
       </c>
@@ -1905,19 +2088,25 @@
         <v>171</v>
       </c>
       <c r="C2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
+      </c>
+      <c r="E2" s="5">
+        <v>4.3</v>
       </c>
       <c r="F2" t="s">
+        <v>250</v>
+      </c>
+      <c r="G2" t="s">
         <v>34</v>
       </c>
-      <c r="G2" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H2" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>172</v>
       </c>
@@ -1925,19 +2114,20 @@
         <v>174</v>
       </c>
       <c r="C3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="F3" t="s">
+        <v>204</v>
+      </c>
+      <c r="E3" s="5"/>
+      <c r="G3" t="s">
         <v>34</v>
       </c>
-      <c r="G3" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>175</v>
       </c>
@@ -1945,19 +2135,25 @@
         <v>173</v>
       </c>
       <c r="C4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D4" t="s">
-        <v>185</v>
+        <v>184</v>
+      </c>
+      <c r="E4" t="s">
+        <v>184</v>
       </c>
       <c r="F4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G4" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+      <c r="H4" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
@@ -1965,20 +2161,25 @@
         <v>3</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3" t="s">
-        <v>227</v>
+        <v>205</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="F5" t="s">
+        <v>252</v>
       </c>
       <c r="G5" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="H5" s="3" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -1986,20 +2187,21 @@
         <v>6</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>207</v>
-      </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3" t="s">
-        <v>227</v>
-      </c>
+        <v>206</v>
+      </c>
+      <c r="E6" s="5"/>
+      <c r="F6" s="3"/>
       <c r="G6" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="H6" s="3" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
@@ -2007,20 +2209,25 @@
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="E7" s="3"/>
+        <v>204</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>253</v>
+      </c>
       <c r="F7" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="H7" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="G7" s="3" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>176</v>
       </c>
@@ -2028,20 +2235,25 @@
         <v>177</v>
       </c>
       <c r="C8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D8" t="s">
-        <v>185</v>
-      </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
+      </c>
+      <c r="E8" t="s">
+        <v>184</v>
+      </c>
+      <c r="F8" t="s">
+        <v>184</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
@@ -2049,20 +2261,25 @@
         <v>9</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="E9" s="3"/>
+        <v>205</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>255</v>
+      </c>
       <c r="F9" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="H9" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="G9" s="3" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
@@ -2070,20 +2287,25 @@
         <v>15</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>208</v>
-      </c>
-      <c r="E10" s="3"/>
+        <v>207</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>257</v>
+      </c>
       <c r="F10" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="G10" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="G10" s="3" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H10" s="3" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
@@ -2091,20 +2313,21 @@
         <v>16</v>
       </c>
       <c r="C11" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>243</v>
-      </c>
       <c r="E11" s="3"/>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="3"/>
+      <c r="G11" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="G11" s="3" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H11" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>12</v>
       </c>
@@ -2112,20 +2335,25 @@
         <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="E12" s="3"/>
+        <v>204</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>259</v>
+      </c>
       <c r="F12" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="G12" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="G12" s="3" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H12" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>13</v>
       </c>
@@ -2133,20 +2361,25 @@
         <v>18</v>
       </c>
       <c r="C13" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="E13" s="3"/>
+        <v>204</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>251</v>
+      </c>
       <c r="F13" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="G13" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="G13" s="3" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H13" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>14</v>
       </c>
@@ -2154,20 +2387,25 @@
         <v>19</v>
       </c>
       <c r="C14" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="E14" s="3"/>
+        <v>204</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>261</v>
+      </c>
       <c r="F14" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="G14" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="G14" s="3" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H14" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>178</v>
       </c>
@@ -2175,20 +2413,25 @@
         <v>179</v>
       </c>
       <c r="C15" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D15" t="s">
-        <v>185</v>
-      </c>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
+      </c>
+      <c r="E15" t="s">
+        <v>184</v>
+      </c>
+      <c r="F15" t="s">
+        <v>184</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>20</v>
       </c>
@@ -2196,20 +2439,25 @@
         <v>21</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="E16" s="3"/>
+        <v>205</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>263</v>
+      </c>
       <c r="F16" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="H16" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="G16" s="3" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>180</v>
       </c>
@@ -2217,20 +2465,25 @@
         <v>181</v>
       </c>
       <c r="C17" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D17" t="s">
-        <v>185</v>
-      </c>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
+      </c>
+      <c r="E17" t="s">
+        <v>184</v>
+      </c>
+      <c r="F17" t="s">
+        <v>184</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>22</v>
       </c>
@@ -2238,20 +2491,21 @@
         <v>23</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="E18" s="5"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="H18" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="G18" s="3" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>24</v>
       </c>
@@ -2259,20 +2513,25 @@
         <v>27</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="E19" s="3"/>
+        <v>208</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>255</v>
+      </c>
       <c r="F19" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="G19" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="G19" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H19" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>25</v>
       </c>
@@ -2280,20 +2539,25 @@
         <v>28</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="E20" s="3"/>
+        <v>212</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>265</v>
+      </c>
       <c r="F20" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="G20" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="G20" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="H20" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>26</v>
       </c>
@@ -2301,20 +2565,25 @@
         <v>29</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="E21" s="3"/>
+        <v>207</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>267</v>
+      </c>
       <c r="F21" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="G21" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="G21" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H21" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>30</v>
       </c>
@@ -2322,20 +2591,25 @@
         <v>31</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="E22" s="3"/>
+        <v>209</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>269</v>
+      </c>
       <c r="F22" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="G22" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="G22" s="3" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H22" s="3" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>32</v>
       </c>
@@ -2343,16 +2617,21 @@
         <v>33</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
+        <v>209</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>270</v>
+      </c>
       <c r="G23" s="3"/>
-    </row>
-    <row r="24" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H23" s="3"/>
+    </row>
+    <row r="24" spans="1:8" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>34</v>
       </c>
@@ -2360,20 +2639,21 @@
         <v>36</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="E24" s="5"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="G24" s="3" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="H24" s="3" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>35</v>
       </c>
@@ -2381,20 +2661,25 @@
         <v>37</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="E25" s="3"/>
+        <v>210</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>251</v>
+      </c>
       <c r="F25" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="G25" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="G25" s="3" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="H25" s="3" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>38</v>
       </c>
@@ -2402,20 +2687,25 @@
         <v>39</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="E26" s="3"/>
+        <v>211</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>271</v>
+      </c>
       <c r="F26" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="G26" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="G26" s="3" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H26" s="3" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>40</v>
       </c>
@@ -2423,20 +2713,25 @@
         <v>44</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="E27" s="3"/>
+        <v>211</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>273</v>
+      </c>
       <c r="F27" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="G27" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="G27" s="3" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="H27" s="3" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>41</v>
       </c>
@@ -2444,20 +2739,25 @@
         <v>45</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="E28" s="3"/>
+        <v>211</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>275</v>
+      </c>
       <c r="F28" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="G28" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="G28" s="3" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H28" s="3" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>42</v>
       </c>
@@ -2465,20 +2765,25 @@
         <v>46</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="E29" s="3"/>
+        <v>211</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>277</v>
+      </c>
       <c r="F29" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="G29" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="G29" s="3" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H29" s="3" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>43</v>
       </c>
@@ -2486,20 +2791,25 @@
         <v>47</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="E30" s="3"/>
+        <v>211</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>279</v>
+      </c>
       <c r="F30" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="G30" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="G30" s="3" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H30" s="3" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>48</v>
       </c>
@@ -2507,20 +2817,25 @@
         <v>51</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="E31" s="3"/>
+        <v>204</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>281</v>
+      </c>
       <c r="F31" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="G31" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="G31" s="3" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H31" s="3" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>49</v>
       </c>
@@ -2528,16 +2843,17 @@
         <v>52</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="E32" s="3"/>
+        <v>212</v>
+      </c>
+      <c r="E32" s="5"/>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
-    </row>
-    <row r="33" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H32" s="3"/>
+    </row>
+    <row r="33" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>50</v>
       </c>
@@ -2545,20 +2861,25 @@
         <v>53</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="E33" s="3"/>
+        <v>208</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>255</v>
+      </c>
       <c r="F33" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="G33" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="G33" s="3" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="H33" s="3" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>56</v>
       </c>
@@ -2566,20 +2887,25 @@
         <v>54</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="E34" s="3"/>
+        <v>208</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>255</v>
+      </c>
       <c r="F34" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="G34" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="G34" s="3" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H34" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>57</v>
       </c>
@@ -2587,20 +2913,25 @@
         <v>55</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="E35" s="3"/>
+        <v>208</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>251</v>
+      </c>
       <c r="F35" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="G35" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="G35" s="3" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H35" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>58</v>
       </c>
@@ -2608,20 +2939,25 @@
         <v>59</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="E36" s="3"/>
+        <v>214</v>
+      </c>
+      <c r="E36" s="5">
+        <v>4.5999999999999996</v>
+      </c>
       <c r="F36" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="G36" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="G36" s="3" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H36" s="3" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>60</v>
       </c>
@@ -2629,20 +2965,25 @@
         <v>66</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="E37" s="3"/>
+        <v>213</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>286</v>
+      </c>
       <c r="F37" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="G37" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="G37" s="3" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="H37" s="3" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>61</v>
       </c>
@@ -2650,20 +2991,25 @@
         <v>67</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="E38" s="3"/>
+        <v>213</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>287</v>
+      </c>
       <c r="F38" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="G38" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G38" s="3" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="H38" s="3" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>62</v>
       </c>
@@ -2671,20 +3017,25 @@
         <v>68</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="E39" s="3"/>
+        <v>214</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>287</v>
+      </c>
       <c r="F39" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="G39" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="G39" s="3" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H39" s="3" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>63</v>
       </c>
@@ -2692,20 +3043,21 @@
         <v>69</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="E40" s="5"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="G40" s="3" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="H40" s="3" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>64</v>
       </c>
@@ -2713,20 +3065,25 @@
         <v>70</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="E41" s="3"/>
+        <v>215</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>286</v>
+      </c>
       <c r="F41" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="G41" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="G41" s="3" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H41" s="3" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>65</v>
       </c>
@@ -2734,20 +3091,25 @@
         <v>71</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="E42" s="3"/>
+        <v>215</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>290</v>
+      </c>
       <c r="F42" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="G42" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="G42" s="3" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H42" s="3" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>73</v>
       </c>
@@ -2755,20 +3117,21 @@
         <v>72</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="E43" s="3"/>
-      <c r="F43" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="E43" s="5"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G43" s="3" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H43" s="3" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>75</v>
       </c>
@@ -2776,20 +3139,21 @@
         <v>74</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="E44" s="3"/>
-      <c r="F44" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="E44" s="5"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G44" s="3" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H44" s="3" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>77</v>
       </c>
@@ -2797,20 +3161,21 @@
         <v>76</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="E45" s="3"/>
-      <c r="F45" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="E45" s="5"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="G45" s="3" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H45" s="3" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>78</v>
       </c>
@@ -2818,20 +3183,21 @@
         <v>79</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="E46" s="3"/>
-      <c r="F46" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="E46" s="5"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="G46" s="3" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="H46" s="3" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>80</v>
       </c>
@@ -2839,20 +3205,21 @@
         <v>81</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="E47" s="3"/>
-      <c r="F47" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="E47" s="5"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="G47" s="3" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H47" s="3" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>82</v>
       </c>
@@ -2860,20 +3227,21 @@
         <v>85</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="E48" s="3"/>
-      <c r="F48" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="E48" s="5"/>
+      <c r="F48" s="3"/>
+      <c r="G48" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="G48" s="3" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="H48" s="3" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>83</v>
       </c>
@@ -2881,20 +3249,21 @@
         <v>86</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="E49" s="3"/>
-      <c r="F49" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="E49" s="5"/>
+      <c r="F49" s="3"/>
+      <c r="G49" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="G49" s="3" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="H49" s="3" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>84</v>
       </c>
@@ -2902,20 +3271,21 @@
         <v>87</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="E50" s="3"/>
-      <c r="F50" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="E50" s="5"/>
+      <c r="F50" s="3"/>
+      <c r="G50" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="G50" s="3" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="H50" s="3" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>89</v>
       </c>
@@ -2923,20 +3293,21 @@
         <v>88</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="E51" s="3"/>
-      <c r="F51" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="E51" s="5"/>
+      <c r="F51" s="3"/>
+      <c r="G51" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="H51" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="G51" s="3" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:8" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>91</v>
       </c>
@@ -2944,20 +3315,21 @@
         <v>96</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="E52" s="3"/>
-      <c r="F52" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="E52" s="5"/>
+      <c r="F52" s="3"/>
+      <c r="G52" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="G52" s="3" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H52" s="3" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>95</v>
       </c>
@@ -2965,20 +3337,21 @@
         <v>97</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="E53" s="3"/>
-      <c r="F53" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="E53" s="5"/>
+      <c r="F53" s="3"/>
+      <c r="G53" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="G53" s="3" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H53" s="3" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>92</v>
       </c>
@@ -2986,20 +3359,21 @@
         <v>98</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="E54" s="3"/>
-      <c r="F54" s="3" t="s">
-        <v>228</v>
-      </c>
+        <v>218</v>
+      </c>
+      <c r="E54" s="5"/>
+      <c r="F54" s="3"/>
       <c r="G54" s="3" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+        <v>227</v>
+      </c>
+      <c r="H54" s="3" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>93</v>
       </c>
@@ -3007,20 +3381,21 @@
         <v>99</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="E55" s="3"/>
-      <c r="F55" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="E55" s="5"/>
+      <c r="F55" s="3"/>
+      <c r="G55" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="G55" s="3" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="H55" s="3" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>94</v>
       </c>
@@ -3028,20 +3403,21 @@
         <v>90</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="E56" s="3"/>
-      <c r="F56" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="E56" s="5"/>
+      <c r="F56" s="3"/>
+      <c r="G56" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="H56" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="G56" s="3" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:8" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>101</v>
       </c>
@@ -3049,20 +3425,21 @@
         <v>100</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="E57" s="3"/>
-      <c r="F57" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="E57" s="7"/>
+      <c r="F57" s="6"/>
+      <c r="G57" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="G57" s="3" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H57" s="3" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>103</v>
       </c>
@@ -3070,20 +3447,25 @@
         <v>110</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="E58" s="3"/>
+        <v>208</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>255</v>
+      </c>
       <c r="F58" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="G58" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="G58" s="3" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="H58" s="3" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>108</v>
       </c>
@@ -3091,20 +3473,25 @@
         <v>111</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="E59" s="3"/>
+        <v>208</v>
+      </c>
+      <c r="E59" s="5" t="s">
+        <v>255</v>
+      </c>
       <c r="F59" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="G59" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="G59" s="3" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="H59" s="3" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>109</v>
       </c>
@@ -3112,20 +3499,25 @@
         <v>112</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="E60" s="3"/>
+        <v>208</v>
+      </c>
+      <c r="E60" s="5" t="s">
+        <v>251</v>
+      </c>
       <c r="F60" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="G60" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="G60" s="3" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H60" s="3" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>104</v>
       </c>
@@ -3133,20 +3525,25 @@
         <v>113</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>208</v>
-      </c>
-      <c r="E61" s="3"/>
+        <v>207</v>
+      </c>
+      <c r="E61" s="5" t="s">
+        <v>257</v>
+      </c>
       <c r="F61" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="G61" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="G61" s="3" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H61" s="3" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>105</v>
       </c>
@@ -3154,20 +3551,25 @@
         <v>114</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="E62" s="3"/>
+        <v>208</v>
+      </c>
+      <c r="E62" s="5" t="s">
+        <v>284</v>
+      </c>
       <c r="F62" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="G62" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="G62" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H62" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>106</v>
       </c>
@@ -3175,20 +3577,21 @@
         <v>115</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="E63" s="3"/>
-      <c r="F63" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="E63" s="5"/>
+      <c r="F63" s="3"/>
+      <c r="G63" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="G63" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H63" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>107</v>
       </c>
@@ -3196,20 +3599,21 @@
         <v>102</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="E64" s="3"/>
-      <c r="F64" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="E64" s="5"/>
+      <c r="F64" s="3"/>
+      <c r="G64" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="G64" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H64" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>116</v>
       </c>
@@ -3217,20 +3621,21 @@
         <v>136</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="E65" s="3"/>
-      <c r="F65" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="E65" s="5"/>
+      <c r="F65" s="3"/>
+      <c r="G65" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="G65" s="3" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H65" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>117</v>
       </c>
@@ -3238,20 +3643,21 @@
         <v>137</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="E66" s="3"/>
-      <c r="F66" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="E66" s="5"/>
+      <c r="F66" s="3"/>
+      <c r="G66" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="G66" s="3" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H66" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>118</v>
       </c>
@@ -3259,20 +3665,21 @@
         <v>138</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="E67" s="3"/>
-      <c r="F67" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="E67" s="5"/>
+      <c r="F67" s="3"/>
+      <c r="G67" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="G67" s="3" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="H67" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>132</v>
       </c>
@@ -3280,20 +3687,21 @@
         <v>140</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="E68" s="3"/>
-      <c r="F68" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="E68" s="5"/>
+      <c r="F68" s="3"/>
+      <c r="G68" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="G68" s="3" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H68" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>119</v>
       </c>
@@ -3301,20 +3709,21 @@
         <v>139</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="E69" s="3"/>
-      <c r="F69" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="E69" s="5"/>
+      <c r="F69" s="3"/>
+      <c r="G69" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="G69" s="3" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="H69" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>133</v>
       </c>
@@ -3322,20 +3731,21 @@
         <v>141</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="E70" s="3"/>
-      <c r="F70" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="E70" s="5"/>
+      <c r="F70" s="3"/>
+      <c r="G70" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="G70" s="3" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H70" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
         <v>134</v>
       </c>
@@ -3343,20 +3753,21 @@
         <v>142</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="E71" s="3"/>
-      <c r="F71" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="E71" s="5"/>
+      <c r="F71" s="3"/>
+      <c r="G71" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="G71" s="3" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H71" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
         <v>135</v>
       </c>
@@ -3364,20 +3775,21 @@
         <v>143</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D72" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="E72" s="3"/>
-      <c r="F72" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="E72" s="5"/>
+      <c r="F72" s="3"/>
+      <c r="G72" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="G72" s="3" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H72" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>120</v>
       </c>
@@ -3385,20 +3797,21 @@
         <v>144</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="E73" s="3"/>
-      <c r="F73" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="E73" s="5"/>
+      <c r="F73" s="3"/>
+      <c r="G73" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="G73" s="3" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H73" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
         <v>121</v>
       </c>
@@ -3406,20 +3819,21 @@
         <v>145</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D74" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="E74" s="3"/>
-      <c r="F74" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="E74" s="5"/>
+      <c r="F74" s="3"/>
+      <c r="G74" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="G74" s="3" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H74" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>122</v>
       </c>
@@ -3427,20 +3841,21 @@
         <v>146</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D75" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="E75" s="3"/>
-      <c r="F75" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="E75" s="5"/>
+      <c r="F75" s="3"/>
+      <c r="G75" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="G75" s="3" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H75" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
         <v>123</v>
       </c>
@@ -3448,20 +3863,21 @@
         <v>147</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D76" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="E76" s="3"/>
-      <c r="F76" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="E76" s="5"/>
+      <c r="F76" s="3"/>
+      <c r="G76" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="G76" s="3" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H76" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
         <v>124</v>
       </c>
@@ -3469,20 +3885,21 @@
         <v>148</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D77" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="E77" s="3"/>
-      <c r="F77" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="E77" s="5"/>
+      <c r="F77" s="3"/>
+      <c r="G77" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="G77" s="3" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H77" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
         <v>125</v>
       </c>
@@ -3490,20 +3907,21 @@
         <v>149</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D78" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="E78" s="3"/>
-      <c r="F78" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="E78" s="5"/>
+      <c r="F78" s="3"/>
+      <c r="G78" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="G78" s="3" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H78" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
         <v>126</v>
       </c>
@@ -3511,20 +3929,21 @@
         <v>150</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D79" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="E79" s="3"/>
-      <c r="F79" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="E79" s="5"/>
+      <c r="F79" s="3"/>
+      <c r="G79" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="G79" s="3" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H79" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
         <v>127</v>
       </c>
@@ -3532,20 +3951,21 @@
         <v>151</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D80" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="E80" s="3"/>
-      <c r="F80" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="E80" s="5"/>
+      <c r="F80" s="3"/>
+      <c r="G80" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="G80" s="3" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H80" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
         <v>128</v>
       </c>
@@ -3553,20 +3973,21 @@
         <v>152</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D81" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="E81" s="3"/>
-      <c r="F81" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="E81" s="5"/>
+      <c r="F81" s="3"/>
+      <c r="G81" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="G81" s="3" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H81" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
         <v>129</v>
       </c>
@@ -3574,20 +3995,21 @@
         <v>153</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D82" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="E82" s="3"/>
-      <c r="F82" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="E82" s="5"/>
+      <c r="F82" s="3"/>
+      <c r="G82" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="G82" s="3" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H82" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
         <v>130</v>
       </c>
@@ -3595,20 +4017,21 @@
         <v>154</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D83" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="E83" s="3"/>
-      <c r="F83" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="E83" s="5"/>
+      <c r="F83" s="3"/>
+      <c r="G83" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="G83" s="3" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H83" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
         <v>131</v>
       </c>
@@ -3616,20 +4039,21 @@
         <v>155</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D84" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="E84" s="3"/>
-      <c r="F84" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="E84" s="5"/>
+      <c r="F84" s="3"/>
+      <c r="G84" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="G84" s="3" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H84" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
         <v>156</v>
       </c>
@@ -3637,20 +4061,21 @@
         <v>163</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D85" s="5" t="s">
-        <v>221</v>
-      </c>
-      <c r="E85" s="3"/>
-      <c r="F85" s="3" t="s">
-        <v>185</v>
-      </c>
+        <v>220</v>
+      </c>
+      <c r="E85" s="5"/>
+      <c r="F85" s="3"/>
       <c r="G85" s="3" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+      <c r="H85" s="3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
         <v>157</v>
       </c>
@@ -3658,20 +4083,21 @@
         <v>164</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D86" s="5" t="s">
-        <v>222</v>
-      </c>
-      <c r="E86" s="3"/>
-      <c r="F86" s="3" t="s">
-        <v>185</v>
-      </c>
+        <v>221</v>
+      </c>
+      <c r="E86" s="5"/>
+      <c r="F86" s="3"/>
       <c r="G86" s="3" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+      <c r="H86" s="3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
         <v>158</v>
       </c>
@@ -3679,20 +4105,21 @@
         <v>165</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D87" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="E87" s="3"/>
-      <c r="F87" s="3" t="s">
-        <v>185</v>
-      </c>
+        <v>222</v>
+      </c>
+      <c r="E87" s="5"/>
+      <c r="F87" s="3"/>
       <c r="G87" s="3" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+      <c r="H87" s="3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
         <v>159</v>
       </c>
@@ -3700,20 +4127,21 @@
         <v>166</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D88" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="E88" s="3"/>
-      <c r="F88" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="E88" s="5"/>
+      <c r="F88" s="3"/>
+      <c r="G88" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G88" s="3" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H88" s="3" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
         <v>160</v>
       </c>
@@ -3721,20 +4149,25 @@
         <v>167</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D89" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="E89" s="3"/>
+        <v>215</v>
+      </c>
+      <c r="E89" s="5" t="s">
+        <v>290</v>
+      </c>
       <c r="F89" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="G89" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G89" s="3" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H89" s="3" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
         <v>161</v>
       </c>
@@ -3742,20 +4175,25 @@
         <v>168</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D90" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="E90" s="3"/>
+        <v>215</v>
+      </c>
+      <c r="E90" s="5" t="s">
+        <v>282</v>
+      </c>
       <c r="F90" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="G90" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G90" s="3" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H90" s="3" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
         <v>162</v>
       </c>
@@ -3763,17 +4201,22 @@
         <v>169</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D91" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="E91" s="3"/>
+        <v>215</v>
+      </c>
+      <c r="E91" s="5" t="s">
+        <v>295</v>
+      </c>
       <c r="F91" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="G91" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G91" s="3" t="s">
-        <v>240</v>
+      <c r="H91" s="3" t="s">
+        <v>239</v>
       </c>
     </row>
   </sheetData>

</xml_diff>